<commit_message>
Add list of statbank tables to docs
</commit_message>
<xml_diff>
--- a/docs/DCD_DataSheet.xlsx
+++ b/docs/DCD_DataSheet.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/losullivan/Documents/repos/bcd-dd-v2.1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/losullivan/Documents/repos/bcd-dd-v2.1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="1560" yWindow="700" windowWidth="32180" windowHeight="18940"/>
+    <workbookView xWindow="1560" yWindow="700" windowWidth="32180" windowHeight="18940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Landing Page" sheetId="2" r:id="rId1"/>
-    <sheet name="Themes Page" sheetId="1" r:id="rId2"/>
+    <sheet name="Statbank" sheetId="3" r:id="rId2"/>
+    <sheet name="discontinued_politcal football" sheetId="4" r:id="rId3"/>
+    <sheet name="Themes Page" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="166">
   <si>
     <t>Chart No</t>
   </si>
@@ -404,13 +406,148 @@
   </si>
   <si>
     <t>Rename File?</t>
+  </si>
+  <si>
+    <t>CLIMATE</t>
+  </si>
+  <si>
+    <t>Google Table</t>
+  </si>
+  <si>
+    <t>JSON table</t>
+  </si>
+  <si>
+    <t>Key Tables</t>
+  </si>
+  <si>
+    <t>MTM01 - Rainfall by Meteorological Weather Station, Month and Statistic (1958M01-2019M12) - Modified on 06/01/2020</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>JSON</t>
+  </si>
+  <si>
+    <t>MTM02 - Temperature by Meteorological Weather Station, Month and Statistic (1958M01-2019M12) - Modified on 06/01/2020</t>
+  </si>
+  <si>
+    <t>MTM03 - Sunshine by Meteorological Weather Station, Month and Statistic (1958M01-2019M12) - Modified on 06/01/2020</t>
+  </si>
+  <si>
+    <t>Current Tables</t>
+  </si>
+  <si>
+    <t>MTM04 - Wind, Maximum Gale Gust (&gt;33.5 Knots) by Meteorological Weather Station and Month (1958M01-2019M12) - Modified on 06/01/2020</t>
+  </si>
+  <si>
+    <t>ICA77 - When Persons last used the Internet by Region, Frequency of Use and Year (2017-2019) - Modified on 24/10/2019</t>
+  </si>
+  <si>
+    <t>ICT USAGE BY ENTERPRISES, HOUSEHOLDS AND PERSONS</t>
+  </si>
+  <si>
+    <t>ICA55 - Persons aged 18 years and over by Purchases Made Online, Region and Year (2011-2019) - Modified on 24/10/2019</t>
+  </si>
+  <si>
+    <t>ICA79 - How often Persons used the Internet by Frequency of Use, Region and Year (2017-2019) - Modified on 24/10/2019</t>
+  </si>
+  <si>
+    <t>ICA46 - Households who have Internet but do not have Broadband Connection by Household Composition, Year and Statistic (2007-2009) - Modified on 02/12/2011</t>
+  </si>
+  <si>
+    <t>ICA47 - Households who have Internet but do not have Broadband Connection by Persons Employed in Household, Year and Statistic (2007-2009) - Modified on 02/12/2011</t>
+  </si>
+  <si>
+    <t>ICA48 - Households who have Internet but do not have Broadband Connection by Population, Year and Statistic (2007-2009) - Modified on 02/12/2011</t>
+  </si>
+  <si>
+    <t>ICA49 - Households who have Internet but do not have Broadband Connection by Region, Year and Statistic (2007-2009) - Modified on 02/12/2011</t>
+  </si>
+  <si>
+    <t>HOUSE PRICES</t>
+  </si>
+  <si>
+    <t>HPM02 - Residential Dwelling Property Transactions by County, Dwelling Status, Stamp Duty Event, Type of Buyer, Type of Sale, Month and Statistic (2010M01-2019M11) - Modified on 15/01/2020</t>
+  </si>
+  <si>
+    <t>HPM03 - Market-based Household Purchases of Residential Dwellings by Dwelling Status, Stamp Duty Event, RPPI Region, Type of Buyer, Month and Statistic (2010M01-2019M11) - Modified on 15/01/2020</t>
+  </si>
+  <si>
+    <t>HPM04 - Market-based Household Purchases of Residential Dwellings by Dwelling Status, Eircode Output, Stamp Duty Event, Type of Buyer, Month and Statistic (2010M01-2019M11) - Modified on 15/01/2020</t>
+  </si>
+  <si>
+    <t>HPM05 - Market-based Household Purchases of Residential Dwellings by Type of Dwelling, Dwelling Status, Stamp Duty Event, RPPI Region, Month and Statistic (2010M01-2019M11) - Modified on 15/01/2020</t>
+  </si>
+  <si>
+    <t>HPM06 - Residential Property Price Index by Type of Residential Property, Month and Statistic (2005M01-2019M11) - Modified on 15/01/2020</t>
+  </si>
+  <si>
+    <t>HPA02 - Residential Dwelling Property Transactions by County, Dwelling Status, Stamp Duty Event, Type of Buyer, Type of Sale, Year and Statistic (2010-2018) - Modified on 13/02/2019</t>
+  </si>
+  <si>
+    <t>HPA03 - Market-based Household Purchases of Residential Dwellings by Dwelling Status, Stamp Duty Event, RPPI Region, Type of Buyer, Year and Statistic (2010-2018) - Modified on 13/02/2019</t>
+  </si>
+  <si>
+    <t>HPA04 - Market-based Household Purchases of Residential Dwellings by Dwelling Status, Eircode Output, Stamp Duty Event, Type of Buyer, Year and Statistic (2010-2018) - Modified on 13/02/2019</t>
+  </si>
+  <si>
+    <t>HPA05 - Market-based Household Purchases of Residential Dwellings by Type of Dwelling, Dwelling Status, Stamp Duty Event, RPPI Region, Year and Statistic (2010-2018) - Modified on 13/02/2019</t>
+  </si>
+  <si>
+    <t>HPA06 - Residential Property Price Index by Type of Residential Property, Year and Statistic (2005-2018) - Modified on 13/02/2019</t>
+  </si>
+  <si>
+    <t>COUNTY INCOMES AND REGIONAL ACCOUNTS</t>
+  </si>
+  <si>
+    <t>CIA02 - Estimates of Household Income by County and Region, Year and Statistic (2000-2016) - Modified on 02/04/2019</t>
+  </si>
+  <si>
+    <t>RAA06 - Gross Value Addded by Region, Year and Statistic (2000-2016) - Modified on 03/04/2019</t>
+  </si>
+  <si>
+    <t>CIA01 - Estimates of Household Income by County and Region, Year and Statistic (2000-2015) - Modified on 26/02/2018</t>
+  </si>
+  <si>
+    <t>RAA01 - Gross Value Added (GVA) by Region, Year and Statistic (2000-2015) - Modified on 26/02/2018</t>
+  </si>
+  <si>
+    <t>GOAL 1 - NO POVERTY</t>
+  </si>
+  <si>
+    <t>G0101 - SDG 1.1.1 Proportion of the Population in Consistent Poverty by NUTS 3 Regions and Year (2004-2017) - Modified on 28/03/2019</t>
+  </si>
+  <si>
+    <t>G0102 - SDG 1.2.1 Proportion of the Population Living below the National Poverty Line by NUTS 3 Regions and Year (2004-2017) - Modified on 28/03/2019</t>
+  </si>
+  <si>
+    <t>G0103 - SDG 1.2.2 Deprivation Rate by NUTS 3 Regions and Year (2004-2017) - Modified on 28/03/2019</t>
+  </si>
+  <si>
+    <t>G0104 - SDG 1.3.1 Proportion of the population receiving Social Welfare Payments by County, Year and Statistic (2007-2016) - Modified on 28/03/2019</t>
+  </si>
+  <si>
+    <t>G0105 - SDG 1.4.1 Dwelling Facilities by NUTS 3 Regions, Year and Statistic (2016-2016) - Modified on 19/02/2019</t>
+  </si>
+  <si>
+    <t>G0106 - SDG 1.4.1 Dwelling Facilities by County, Year and Statistic (2016-2016) - Modified on 19/02/2019</t>
+  </si>
+  <si>
+    <t>G0107 - SDG 1.4.2 Proportion of total adult population with secure tenure rights to land by NUTS 3 Regions, Year and Statistic (2016-2016) - Modified on 21/02/2019</t>
+  </si>
+  <si>
+    <t>G0108 - SDG 1.4.2 Proportion of total adult population with secure tenure rights to land by County, Year and Statistic (2016-2016) - Modified on 21/02/2019</t>
+  </si>
+  <si>
+    <t>G0112 - SDG 1.5.4 Proportion of local governments that adopt and implement local disaster risk reduction strategies in line with national disaster risk reduction strategies by State and Year (2018-2018) - Modified on 11/04/2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,6 +623,27 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="17.600000000000001"/>
+      <color rgb="FF1D1D1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF4C4C4C"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF1D1D1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -567,7 +725,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -605,6 +763,9 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="60% - Accent6" xfId="7" builtinId="52"/>
@@ -957,7 +1118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A17:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="B16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -1128,6 +1289,638 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72:C72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="105.5" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="B1" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="20"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="21"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="21"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="21"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="21"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A45" s="19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A47" s="20"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="21"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="21"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="21"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="21"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A58" s="19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A60" s="20"/>
+      <c r="B60" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="21"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A61:A62"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A8" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId2"/>
+    <hyperlink ref="C8" r:id="rId3"/>
+    <hyperlink ref="A9" r:id="rId4"/>
+    <hyperlink ref="B9" r:id="rId5"/>
+    <hyperlink ref="C9" r:id="rId6"/>
+    <hyperlink ref="A10" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="A13" r:id="rId10"/>
+    <hyperlink ref="B13" r:id="rId11"/>
+    <hyperlink ref="C13" r:id="rId12"/>
+    <hyperlink ref="A19" r:id="rId13"/>
+    <hyperlink ref="B19" r:id="rId14"/>
+    <hyperlink ref="C19" r:id="rId15"/>
+    <hyperlink ref="A24" r:id="rId16"/>
+    <hyperlink ref="B24" r:id="rId17"/>
+    <hyperlink ref="C24" r:id="rId18"/>
+    <hyperlink ref="A20" r:id="rId19"/>
+    <hyperlink ref="B20" r:id="rId20"/>
+    <hyperlink ref="C20" r:id="rId21"/>
+    <hyperlink ref="A32" r:id="rId22"/>
+    <hyperlink ref="B32" r:id="rId23"/>
+    <hyperlink ref="C32" r:id="rId24"/>
+    <hyperlink ref="A33" r:id="rId25"/>
+    <hyperlink ref="B33" r:id="rId26"/>
+    <hyperlink ref="C33" r:id="rId27"/>
+    <hyperlink ref="A34" r:id="rId28"/>
+    <hyperlink ref="B34" r:id="rId29"/>
+    <hyperlink ref="C34" r:id="rId30"/>
+    <hyperlink ref="A35" r:id="rId31"/>
+    <hyperlink ref="B35" r:id="rId32"/>
+    <hyperlink ref="C35" r:id="rId33"/>
+    <hyperlink ref="A36" r:id="rId34"/>
+    <hyperlink ref="B36" r:id="rId35"/>
+    <hyperlink ref="C36" r:id="rId36"/>
+    <hyperlink ref="A38" r:id="rId37"/>
+    <hyperlink ref="B38" r:id="rId38"/>
+    <hyperlink ref="C38" r:id="rId39"/>
+    <hyperlink ref="A39" r:id="rId40"/>
+    <hyperlink ref="B39" r:id="rId41"/>
+    <hyperlink ref="C39" r:id="rId42"/>
+    <hyperlink ref="A40" r:id="rId43"/>
+    <hyperlink ref="B40" r:id="rId44"/>
+    <hyperlink ref="C40" r:id="rId45"/>
+    <hyperlink ref="A41" r:id="rId46"/>
+    <hyperlink ref="B41" r:id="rId47"/>
+    <hyperlink ref="C41" r:id="rId48"/>
+    <hyperlink ref="A42" r:id="rId49"/>
+    <hyperlink ref="B42" r:id="rId50"/>
+    <hyperlink ref="C42" r:id="rId51"/>
+    <hyperlink ref="A50" r:id="rId52"/>
+    <hyperlink ref="B50" r:id="rId53"/>
+    <hyperlink ref="C50" r:id="rId54"/>
+    <hyperlink ref="A51" r:id="rId55"/>
+    <hyperlink ref="B51" r:id="rId56"/>
+    <hyperlink ref="C51" r:id="rId57"/>
+    <hyperlink ref="A54" r:id="rId58"/>
+    <hyperlink ref="B54" r:id="rId59"/>
+    <hyperlink ref="C54" r:id="rId60"/>
+    <hyperlink ref="A55" r:id="rId61"/>
+    <hyperlink ref="B55" r:id="rId62"/>
+    <hyperlink ref="C55" r:id="rId63"/>
+    <hyperlink ref="A63" r:id="rId64"/>
+    <hyperlink ref="B63" r:id="rId65"/>
+    <hyperlink ref="C63" r:id="rId66"/>
+    <hyperlink ref="A64" r:id="rId67"/>
+    <hyperlink ref="B64" r:id="rId68"/>
+    <hyperlink ref="C64" r:id="rId69"/>
+    <hyperlink ref="A65" r:id="rId70"/>
+    <hyperlink ref="B65" r:id="rId71"/>
+    <hyperlink ref="C65" r:id="rId72"/>
+    <hyperlink ref="A66" r:id="rId73"/>
+    <hyperlink ref="B66" r:id="rId74"/>
+    <hyperlink ref="C66" r:id="rId75"/>
+    <hyperlink ref="A67" r:id="rId76"/>
+    <hyperlink ref="B67" r:id="rId77"/>
+    <hyperlink ref="C67" r:id="rId78"/>
+    <hyperlink ref="A68" r:id="rId79"/>
+    <hyperlink ref="B68" r:id="rId80"/>
+    <hyperlink ref="C68" r:id="rId81"/>
+    <hyperlink ref="A69" r:id="rId82"/>
+    <hyperlink ref="B69" r:id="rId83"/>
+    <hyperlink ref="C69" r:id="rId84"/>
+    <hyperlink ref="A70" r:id="rId85"/>
+    <hyperlink ref="B70" r:id="rId86"/>
+    <hyperlink ref="C70" r:id="rId87"/>
+    <hyperlink ref="A72" r:id="rId88"/>
+    <hyperlink ref="B72" r:id="rId89"/>
+    <hyperlink ref="C72" r:id="rId90"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="71.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="C4" r:id="rId6"/>
+    <hyperlink ref="A5" r:id="rId7"/>
+    <hyperlink ref="B5" r:id="rId8"/>
+    <hyperlink ref="C5" r:id="rId9"/>
+    <hyperlink ref="A6" r:id="rId10"/>
+    <hyperlink ref="B6" r:id="rId11"/>
+    <hyperlink ref="C6" r:id="rId12"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add to list of statbank tables
</commit_message>
<xml_diff>
--- a/docs/DCD_DataSheet.xlsx
+++ b/docs/DCD_DataSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="700" windowWidth="32180" windowHeight="18940" activeTab="1"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="19420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Landing Page" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="189">
   <si>
     <t>Chart No</t>
   </si>
@@ -417,9 +417,6 @@
     <t>JSON table</t>
   </si>
   <si>
-    <t>Key Tables</t>
-  </si>
-  <si>
     <t>MTM01 - Rainfall by Meteorological Weather Station, Month and Statistic (1958M01-2019M12) - Modified on 06/01/2020</t>
   </si>
   <si>
@@ -435,9 +432,6 @@
     <t>MTM03 - Sunshine by Meteorological Weather Station, Month and Statistic (1958M01-2019M12) - Modified on 06/01/2020</t>
   </si>
   <si>
-    <t>Current Tables</t>
-  </si>
-  <si>
     <t>MTM04 - Wind, Maximum Gale Gust (&gt;33.5 Knots) by Meteorological Weather Station and Month (1958M01-2019M12) - Modified on 06/01/2020</t>
   </si>
   <si>
@@ -541,13 +535,88 @@
   </si>
   <si>
     <t>G0112 - SDG 1.5.4 Proportion of local governments that adopt and implement local disaster risk reduction strategies in line with national disaster risk reduction strategies by State and Year (2018-2018) - Modified on 11/04/2019</t>
+  </si>
+  <si>
+    <t>ED123 - Nationality of Pupils attending Primary School by County, Nationality of Pupil and Year (2017-2019) - Modified on 28/06/2019</t>
+  </si>
+  <si>
+    <t>DEPARTMENT OF EDUCATION AND SKILLS</t>
+  </si>
+  <si>
+    <t>ED126 - Pupils attending Mainstream Primary Schools by County, Ethos, Year and Statistic (2017-2019) - Modified on 27/06/2019</t>
+  </si>
+  <si>
+    <t>ED133 - Pupils enrolled in Second-Level Schools by County, Nationality of Pupil and Year (2000-2019) - Modified on 27/06/2019</t>
+  </si>
+  <si>
+    <t>EDA43 - Early Start Pre-school Programmes by County, Year and Statistic (2000-2019) - Modified on 19/06/2019</t>
+  </si>
+  <si>
+    <t>EDA56 - National Schools by County, Year and Statistic (1995-2019) - Modified on 03/07/2019</t>
+  </si>
+  <si>
+    <t>EDA57 - National School Pupils by County, School Programme, Year and Statistic (1995-2019) - Modified on 19/06/2019</t>
+  </si>
+  <si>
+    <t>EDA69 - Second Level Schools and Pupils by County, Type of School, Year and Statistic (2000-2019) - Modified on 19/06/2019</t>
+  </si>
+  <si>
+    <t>EDA98 - Students from Ireland and Northern Ireland by County of Origin, County of Study and Year (2000-2017) - Modified on 19/12/2017</t>
+  </si>
+  <si>
+    <t>EDA99 - Students Enrolled in and Entrants to Third Level Courses by Institution, Year and Statistic (2000-2017) - Modified on 19/12/2017</t>
+  </si>
+  <si>
+    <t>RESIDENTIAL TENANCIES BOARD (PRTB)</t>
+  </si>
+  <si>
+    <t>RIA02 - RTB Average Monthly Rent Report by Number of Bedrooms, Property Type, Location and Year (2008-2018) - Modified on 19/12/2019</t>
+  </si>
+  <si>
+    <t>RIH02 - RTB Average Monthly Rent Report by Number of Bedrooms, Property Type, Location and HalfYear (2008H1-2019H1) - Modified on 19/12/2019</t>
+  </si>
+  <si>
+    <t>RIQ02 - RTB Average Monthly Rent Report by Number of Bedrooms, Property Type, Location and Quarter (2007Q4-2019Q3) - Modified on 19/12/2019</t>
+  </si>
+  <si>
+    <t>DEPARTMENT OF HOUSING, PLANNING, COMMUNITY AND LOCAL GOVERNMENT</t>
+  </si>
+  <si>
+    <t>HSA10 - New House Registrations by County and Year (1978-2018) - Modified on 05/03/2019</t>
+  </si>
+  <si>
+    <t>HSM13 - Commencement Notices by Local Authority, Residential Units Commenced and Month (2016M04-2019M09) - Modified on 12/11/2019</t>
+  </si>
+  <si>
+    <t>HSQ10 - New House Registrations by County and Quarter (1994Q1-2019Q3) - Modified on 12/11/2019</t>
+  </si>
+  <si>
+    <t>HSQ13 - Local Authority Loan Arrears by Local Authority, Quarter and Statistic (2015Q4-2019Q2) - Modified on 12/11/2019</t>
+  </si>
+  <si>
+    <t>NATIONAL ROADS AUTHORITY</t>
+  </si>
+  <si>
+    <t>NRA01 - National Road Length by Type of Carriageway and Year (2004-2018) - Modified on 14/11/2019</t>
+  </si>
+  <si>
+    <t>NRA03 - National Route Length by Local Authority, Type of Carriageway and Year (2015-2018) - Modified on 19/11/2019</t>
+  </si>
+  <si>
+    <t>ROA15 - Persons Killed and Injured by County, Year and Statistic (2001-2018) - Modified on 29/10/2019</t>
+  </si>
+  <si>
+    <t>ROA26 - Current Driving Licences by Age Group, Licensing Authority, Year and Statistic (2013-2018) - Modified on 29/10/2019</t>
+  </si>
+  <si>
+    <t>ROA27 - Traffic Collisions and Casualities by County, Year and Statistic (2013-2017) - Modified on 22/11/2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -638,13 +707,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF1D1D1D"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -725,7 +787,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -765,7 +827,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="60% - Accent6" xfId="7" builtinId="52"/>
@@ -1290,10 +1351,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:C72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2 A4:A7 A11:A12 A14:A16 A18 A21:A23 A25:A26 A28:A31 A37 A43:A44 A46:A49 A52:A53 A56:A57 A59 A61:A62 A71 A73:A74 A79 A81 A83 A85 A87 A90 A92:A95 A99:A101 A103:A106 A108 A112:A113 A115:A118 A121:A122 A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1304,543 +1365,728 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>122</v>
+      </c>
       <c r="B1" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C1" s="20" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="23" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+    <row r="2" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
+      <c r="A6" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
+      <c r="A12" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="23" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>133</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A29" s="20"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A28" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="21"/>
+      <c r="A30" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="21"/>
+      <c r="A31" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="23" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="20"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="21"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A48" s="19" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="21"/>
+      <c r="A49" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="21"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A52" s="19" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="21"/>
+      <c r="A53" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="23" x14ac:dyDescent="0.25">
-      <c r="A58" s="19" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A60" s="20"/>
-      <c r="B60" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C60" s="20" t="s">
-        <v>123</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A57" s="19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="21" t="s">
-        <v>124</v>
+      <c r="A61" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="21"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>127</v>
+      <c r="A62" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A61:A62"/>
-  </mergeCells>
+  <dataConsolidate/>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1"/>
-    <hyperlink ref="B8" r:id="rId2"/>
-    <hyperlink ref="C8" r:id="rId3"/>
-    <hyperlink ref="A9" r:id="rId4"/>
-    <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="C9" r:id="rId6"/>
-    <hyperlink ref="A10" r:id="rId7"/>
-    <hyperlink ref="B10" r:id="rId8"/>
-    <hyperlink ref="C10" r:id="rId9"/>
-    <hyperlink ref="A13" r:id="rId10"/>
-    <hyperlink ref="B13" r:id="rId11"/>
-    <hyperlink ref="C13" r:id="rId12"/>
-    <hyperlink ref="A19" r:id="rId13"/>
-    <hyperlink ref="B19" r:id="rId14"/>
-    <hyperlink ref="C19" r:id="rId15"/>
-    <hyperlink ref="A24" r:id="rId16"/>
-    <hyperlink ref="B24" r:id="rId17"/>
-    <hyperlink ref="C24" r:id="rId18"/>
-    <hyperlink ref="A20" r:id="rId19"/>
-    <hyperlink ref="B20" r:id="rId20"/>
-    <hyperlink ref="C20" r:id="rId21"/>
-    <hyperlink ref="A32" r:id="rId22"/>
-    <hyperlink ref="B32" r:id="rId23"/>
-    <hyperlink ref="C32" r:id="rId24"/>
-    <hyperlink ref="A33" r:id="rId25"/>
-    <hyperlink ref="B33" r:id="rId26"/>
-    <hyperlink ref="C33" r:id="rId27"/>
-    <hyperlink ref="A34" r:id="rId28"/>
-    <hyperlink ref="B34" r:id="rId29"/>
-    <hyperlink ref="C34" r:id="rId30"/>
-    <hyperlink ref="A35" r:id="rId31"/>
-    <hyperlink ref="B35" r:id="rId32"/>
-    <hyperlink ref="C35" r:id="rId33"/>
-    <hyperlink ref="A36" r:id="rId34"/>
-    <hyperlink ref="B36" r:id="rId35"/>
-    <hyperlink ref="C36" r:id="rId36"/>
-    <hyperlink ref="A38" r:id="rId37"/>
-    <hyperlink ref="B38" r:id="rId38"/>
-    <hyperlink ref="C38" r:id="rId39"/>
-    <hyperlink ref="A39" r:id="rId40"/>
-    <hyperlink ref="B39" r:id="rId41"/>
-    <hyperlink ref="C39" r:id="rId42"/>
-    <hyperlink ref="A40" r:id="rId43"/>
-    <hyperlink ref="B40" r:id="rId44"/>
-    <hyperlink ref="C40" r:id="rId45"/>
-    <hyperlink ref="A41" r:id="rId46"/>
-    <hyperlink ref="B41" r:id="rId47"/>
-    <hyperlink ref="C41" r:id="rId48"/>
-    <hyperlink ref="A42" r:id="rId49"/>
-    <hyperlink ref="B42" r:id="rId50"/>
-    <hyperlink ref="C42" r:id="rId51"/>
-    <hyperlink ref="A50" r:id="rId52"/>
-    <hyperlink ref="B50" r:id="rId53"/>
-    <hyperlink ref="C50" r:id="rId54"/>
-    <hyperlink ref="A51" r:id="rId55"/>
-    <hyperlink ref="B51" r:id="rId56"/>
-    <hyperlink ref="C51" r:id="rId57"/>
-    <hyperlink ref="A54" r:id="rId58"/>
-    <hyperlink ref="B54" r:id="rId59"/>
-    <hyperlink ref="C54" r:id="rId60"/>
-    <hyperlink ref="A55" r:id="rId61"/>
-    <hyperlink ref="B55" r:id="rId62"/>
-    <hyperlink ref="C55" r:id="rId63"/>
-    <hyperlink ref="A63" r:id="rId64"/>
-    <hyperlink ref="B63" r:id="rId65"/>
-    <hyperlink ref="C63" r:id="rId66"/>
-    <hyperlink ref="A64" r:id="rId67"/>
-    <hyperlink ref="B64" r:id="rId68"/>
-    <hyperlink ref="C64" r:id="rId69"/>
-    <hyperlink ref="A65" r:id="rId70"/>
-    <hyperlink ref="B65" r:id="rId71"/>
-    <hyperlink ref="C65" r:id="rId72"/>
-    <hyperlink ref="A66" r:id="rId73"/>
-    <hyperlink ref="B66" r:id="rId74"/>
-    <hyperlink ref="C66" r:id="rId75"/>
-    <hyperlink ref="A67" r:id="rId76"/>
-    <hyperlink ref="B67" r:id="rId77"/>
-    <hyperlink ref="C67" r:id="rId78"/>
-    <hyperlink ref="A68" r:id="rId79"/>
-    <hyperlink ref="B68" r:id="rId80"/>
-    <hyperlink ref="C68" r:id="rId81"/>
-    <hyperlink ref="A69" r:id="rId82"/>
-    <hyperlink ref="B69" r:id="rId83"/>
-    <hyperlink ref="C69" r:id="rId84"/>
-    <hyperlink ref="A70" r:id="rId85"/>
-    <hyperlink ref="B70" r:id="rId86"/>
-    <hyperlink ref="C70" r:id="rId87"/>
-    <hyperlink ref="A72" r:id="rId88"/>
-    <hyperlink ref="B72" r:id="rId89"/>
-    <hyperlink ref="C72" r:id="rId90"/>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
+    <hyperlink ref="C5" r:id="rId6"/>
+    <hyperlink ref="A6" r:id="rId7"/>
+    <hyperlink ref="C6" r:id="rId8"/>
+    <hyperlink ref="A8" r:id="rId9"/>
+    <hyperlink ref="C8" r:id="rId10"/>
+    <hyperlink ref="A10" r:id="rId11"/>
+    <hyperlink ref="C10" r:id="rId12"/>
+    <hyperlink ref="A9" r:id="rId13"/>
+    <hyperlink ref="C9" r:id="rId14"/>
+    <hyperlink ref="A12" r:id="rId15"/>
+    <hyperlink ref="C12" r:id="rId16"/>
+    <hyperlink ref="A13" r:id="rId17"/>
+    <hyperlink ref="C13" r:id="rId18"/>
+    <hyperlink ref="A14" r:id="rId19"/>
+    <hyperlink ref="C14" r:id="rId20"/>
+    <hyperlink ref="A15" r:id="rId21"/>
+    <hyperlink ref="C15" r:id="rId22"/>
+    <hyperlink ref="A16" r:id="rId23"/>
+    <hyperlink ref="C16" r:id="rId24"/>
+    <hyperlink ref="A17" r:id="rId25"/>
+    <hyperlink ref="C17" r:id="rId26"/>
+    <hyperlink ref="A18" r:id="rId27"/>
+    <hyperlink ref="C18" r:id="rId28"/>
+    <hyperlink ref="A19" r:id="rId29"/>
+    <hyperlink ref="C19" r:id="rId30"/>
+    <hyperlink ref="A20" r:id="rId31"/>
+    <hyperlink ref="C20" r:id="rId32"/>
+    <hyperlink ref="A21" r:id="rId33"/>
+    <hyperlink ref="C21" r:id="rId34"/>
+    <hyperlink ref="A23" r:id="rId35"/>
+    <hyperlink ref="C23" r:id="rId36"/>
+    <hyperlink ref="A24" r:id="rId37"/>
+    <hyperlink ref="C24" r:id="rId38"/>
+    <hyperlink ref="A25" r:id="rId39"/>
+    <hyperlink ref="C25" r:id="rId40"/>
+    <hyperlink ref="A26" r:id="rId41"/>
+    <hyperlink ref="C26" r:id="rId42"/>
+    <hyperlink ref="A29" r:id="rId43"/>
+    <hyperlink ref="C29" r:id="rId44"/>
+    <hyperlink ref="A30" r:id="rId45"/>
+    <hyperlink ref="C30" r:id="rId46"/>
+    <hyperlink ref="A31" r:id="rId47"/>
+    <hyperlink ref="C31" r:id="rId48"/>
+    <hyperlink ref="A32" r:id="rId49"/>
+    <hyperlink ref="C32" r:id="rId50"/>
+    <hyperlink ref="A33" r:id="rId51"/>
+    <hyperlink ref="C33" r:id="rId52"/>
+    <hyperlink ref="A34" r:id="rId53"/>
+    <hyperlink ref="C34" r:id="rId54"/>
+    <hyperlink ref="A35" r:id="rId55"/>
+    <hyperlink ref="C35" r:id="rId56"/>
+    <hyperlink ref="A36" r:id="rId57"/>
+    <hyperlink ref="C36" r:id="rId58"/>
+    <hyperlink ref="A37" r:id="rId59"/>
+    <hyperlink ref="C37" r:id="rId60"/>
+    <hyperlink ref="A39" r:id="rId61"/>
+    <hyperlink ref="C39" r:id="rId62"/>
+    <hyperlink ref="A40" r:id="rId63"/>
+    <hyperlink ref="C40" r:id="rId64"/>
+    <hyperlink ref="A41" r:id="rId65"/>
+    <hyperlink ref="C41" r:id="rId66"/>
+    <hyperlink ref="A42" r:id="rId67"/>
+    <hyperlink ref="C42" r:id="rId68"/>
+    <hyperlink ref="A43" r:id="rId69"/>
+    <hyperlink ref="C43" r:id="rId70"/>
+    <hyperlink ref="A44" r:id="rId71"/>
+    <hyperlink ref="C44" r:id="rId72"/>
+    <hyperlink ref="A45" r:id="rId73"/>
+    <hyperlink ref="C45" r:id="rId74"/>
+    <hyperlink ref="A46" r:id="rId75"/>
+    <hyperlink ref="C46" r:id="rId76"/>
+    <hyperlink ref="A47" r:id="rId77"/>
+    <hyperlink ref="C47" r:id="rId78"/>
+    <hyperlink ref="A49" r:id="rId79"/>
+    <hyperlink ref="C49" r:id="rId80"/>
+    <hyperlink ref="A50" r:id="rId81"/>
+    <hyperlink ref="C50" r:id="rId82"/>
+    <hyperlink ref="A51" r:id="rId83"/>
+    <hyperlink ref="C51" r:id="rId84"/>
+    <hyperlink ref="A53" r:id="rId85"/>
+    <hyperlink ref="C53" r:id="rId86"/>
+    <hyperlink ref="A54" r:id="rId87"/>
+    <hyperlink ref="C54" r:id="rId88"/>
+    <hyperlink ref="A55" r:id="rId89"/>
+    <hyperlink ref="C55" r:id="rId90"/>
+    <hyperlink ref="B58" r:id="rId91"/>
+    <hyperlink ref="C58" r:id="rId92"/>
+    <hyperlink ref="A59" r:id="rId93"/>
+    <hyperlink ref="C59" r:id="rId94"/>
+    <hyperlink ref="A60" r:id="rId95"/>
+    <hyperlink ref="C60" r:id="rId96"/>
+    <hyperlink ref="A61" r:id="rId97"/>
+    <hyperlink ref="C61" r:id="rId98"/>
+    <hyperlink ref="A62" r:id="rId99"/>
+    <hyperlink ref="C62" r:id="rId100"/>
+    <hyperlink ref="A56" r:id="rId101"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1859,46 +2105,46 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Select random table from list
</commit_message>
<xml_diff>
--- a/docs/DCD_DataSheet.xlsx
+++ b/docs/DCD_DataSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="19420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Landing Page" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="239">
   <si>
     <t>Chart No</t>
   </si>
@@ -610,13 +610,163 @@
   </si>
   <si>
     <t>ROA27 - Traffic Collisions and Casualities by County, Year and Statistic (2013-2017) - Modified on 22/11/2019</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/MTM01</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/MTM02</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/MTM03</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/MTM04</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/ICA77</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/ICA79</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/ICA55</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/HPM02</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/HPM03</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/HPM04</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/HPM05</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/HPM06</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/HPA02</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/HPA03</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/HPA04</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/HPA05</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/HPA06</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/CIA02</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/RAA06</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/CIA01</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/RAA01</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/G0101</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/G0102</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/G0103</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/G0104</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/G0105</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/G0106</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/G0107</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/G0108</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/G0112</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/ED123</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/ED126</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/ED133</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/EDA43</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/EDA56</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/EDA57</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/EDA69</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/EDA98</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/EDA99</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/RIA02</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/RIH02</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/RIQ02</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/HSA10</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/HSM13</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/HSQ10</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/NRA01</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/NRA03</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/ROA15</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/ROA26</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/ROA27</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -707,6 +857,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -776,7 +934,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -786,6 +944,8 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -828,12 +988,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="60% - Accent6" xfId="7" builtinId="52"/>
     <cellStyle name="Accent1" xfId="4" builtinId="29"/>
     <cellStyle name="Accent3" xfId="5" builtinId="37"/>
     <cellStyle name="Accent4" xfId="6" builtinId="41"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1353,8 +1515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2 A4:A7 A11:A12 A14:A16 A18 A21:A23 A25:A26 A28:A31 A37 A43:A44 A46:A49 A52:A53 A56:A57 A59 A61:A62 A71 A73:A74 A79 A81 A83 A85 A87 A90 A92:A95 A99:A101 A103:A106 A108 A112:A113 A115:A118 A121:A122 A124"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C28" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1385,7 +1547,7 @@
         <v>125</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>126</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1396,7 +1558,7 @@
         <v>125</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>126</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1407,7 +1569,7 @@
         <v>125</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>126</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1418,7 +1580,7 @@
         <v>125</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>126</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="23" x14ac:dyDescent="0.25">
@@ -1434,7 +1596,7 @@
         <v>125</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>126</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1445,7 +1607,7 @@
         <v>125</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>126</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1456,7 +1618,7 @@
         <v>125</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>126</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="23" x14ac:dyDescent="0.25">
@@ -1472,7 +1634,7 @@
         <v>125</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>126</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1483,7 +1645,7 @@
         <v>125</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>126</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1494,7 +1656,7 @@
         <v>125</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>126</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1505,7 +1667,7 @@
         <v>125</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>126</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1516,7 +1678,7 @@
         <v>125</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>126</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1527,7 +1689,7 @@
         <v>125</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>126</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1538,7 +1700,7 @@
         <v>125</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>126</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1549,7 +1711,7 @@
         <v>125</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>126</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1560,7 +1722,7 @@
         <v>125</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>126</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1571,7 +1733,7 @@
         <v>125</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>126</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="23" x14ac:dyDescent="0.25">
@@ -1587,7 +1749,7 @@
         <v>125</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>126</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1598,7 +1760,7 @@
         <v>125</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>126</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1609,7 +1771,7 @@
         <v>125</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>126</v>
+        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1620,7 +1782,7 @@
         <v>125</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>126</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="23" x14ac:dyDescent="0.25">
@@ -1644,7 +1806,7 @@
         <v>125</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>126</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1655,7 +1817,7 @@
         <v>125</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>126</v>
+        <v>211</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1666,7 +1828,7 @@
         <v>125</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>126</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1677,7 +1839,7 @@
         <v>125</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>126</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1688,7 +1850,7 @@
         <v>125</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>126</v>
+        <v>214</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1699,7 +1861,7 @@
         <v>125</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>126</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1710,7 +1872,7 @@
         <v>125</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>126</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1721,7 +1883,7 @@
         <v>125</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>126</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1732,7 +1894,7 @@
         <v>125</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>126</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="23" x14ac:dyDescent="0.25">
@@ -1748,7 +1910,7 @@
         <v>125</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>126</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1759,7 +1921,7 @@
         <v>125</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>126</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1770,7 +1932,7 @@
         <v>125</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>126</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1781,7 +1943,7 @@
         <v>125</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>126</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1792,7 +1954,7 @@
         <v>125</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>126</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1803,7 +1965,7 @@
         <v>125</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>126</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1814,7 +1976,7 @@
         <v>125</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>126</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1825,7 +1987,7 @@
         <v>125</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>126</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1836,7 +1998,7 @@
         <v>125</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>126</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="23" x14ac:dyDescent="0.25">
@@ -1852,7 +2014,7 @@
         <v>125</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>126</v>
+        <v>228</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1863,7 +2025,7 @@
         <v>125</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>126</v>
+        <v>229</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1874,7 +2036,7 @@
         <v>125</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>126</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="23" x14ac:dyDescent="0.25">
@@ -1890,7 +2052,7 @@
         <v>125</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>126</v>
+        <v>231</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1901,7 +2063,7 @@
         <v>125</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>126</v>
+        <v>232</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1912,7 +2074,7 @@
         <v>125</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>126</v>
+        <v>233</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1933,7 +2095,7 @@
         <v>125</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>126</v>
+        <v>234</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -1944,7 +2106,7 @@
         <v>125</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>126</v>
+        <v>235</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -1955,7 +2117,7 @@
         <v>125</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>126</v>
+        <v>236</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -1966,7 +2128,7 @@
         <v>125</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>126</v>
+        <v>237</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -1977,112 +2139,112 @@
         <v>125</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>126</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId2" display="JSON"/>
     <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="C4" r:id="rId4" display="JSON"/>
     <hyperlink ref="A5" r:id="rId5"/>
-    <hyperlink ref="C5" r:id="rId6"/>
+    <hyperlink ref="C5" r:id="rId6" display="JSON"/>
     <hyperlink ref="A6" r:id="rId7"/>
-    <hyperlink ref="C6" r:id="rId8"/>
+    <hyperlink ref="C6" r:id="rId8" display="JSON"/>
     <hyperlink ref="A8" r:id="rId9"/>
-    <hyperlink ref="C8" r:id="rId10"/>
+    <hyperlink ref="C8" r:id="rId10" display="JSON"/>
     <hyperlink ref="A10" r:id="rId11"/>
-    <hyperlink ref="C10" r:id="rId12"/>
+    <hyperlink ref="C10" r:id="rId12" display="JSON"/>
     <hyperlink ref="A9" r:id="rId13"/>
-    <hyperlink ref="C9" r:id="rId14"/>
+    <hyperlink ref="C9" r:id="rId14" display="JSON"/>
     <hyperlink ref="A12" r:id="rId15"/>
-    <hyperlink ref="C12" r:id="rId16"/>
+    <hyperlink ref="C12" r:id="rId16" display="JSON"/>
     <hyperlink ref="A13" r:id="rId17"/>
-    <hyperlink ref="C13" r:id="rId18"/>
+    <hyperlink ref="C13" r:id="rId18" display="JSON"/>
     <hyperlink ref="A14" r:id="rId19"/>
-    <hyperlink ref="C14" r:id="rId20"/>
+    <hyperlink ref="C14" r:id="rId20" display="JSON"/>
     <hyperlink ref="A15" r:id="rId21"/>
-    <hyperlink ref="C15" r:id="rId22"/>
+    <hyperlink ref="C15" r:id="rId22" display="JSON"/>
     <hyperlink ref="A16" r:id="rId23"/>
-    <hyperlink ref="C16" r:id="rId24"/>
+    <hyperlink ref="C16" r:id="rId24" display="JSON"/>
     <hyperlink ref="A17" r:id="rId25"/>
-    <hyperlink ref="C17" r:id="rId26"/>
+    <hyperlink ref="C17" r:id="rId26" display="JSON"/>
     <hyperlink ref="A18" r:id="rId27"/>
-    <hyperlink ref="C18" r:id="rId28"/>
+    <hyperlink ref="C18" r:id="rId28" display="JSON"/>
     <hyperlink ref="A19" r:id="rId29"/>
-    <hyperlink ref="C19" r:id="rId30"/>
+    <hyperlink ref="C19" r:id="rId30" display="JSON"/>
     <hyperlink ref="A20" r:id="rId31"/>
-    <hyperlink ref="C20" r:id="rId32"/>
+    <hyperlink ref="C20" r:id="rId32" display="JSON"/>
     <hyperlink ref="A21" r:id="rId33"/>
-    <hyperlink ref="C21" r:id="rId34"/>
+    <hyperlink ref="C21" r:id="rId34" display="JSON"/>
     <hyperlink ref="A23" r:id="rId35"/>
-    <hyperlink ref="C23" r:id="rId36"/>
+    <hyperlink ref="C23" r:id="rId36" display="JSON"/>
     <hyperlink ref="A24" r:id="rId37"/>
-    <hyperlink ref="C24" r:id="rId38"/>
+    <hyperlink ref="C24" r:id="rId38" display="JSON"/>
     <hyperlink ref="A25" r:id="rId39"/>
-    <hyperlink ref="C25" r:id="rId40"/>
+    <hyperlink ref="C25" r:id="rId40" display="JSON"/>
     <hyperlink ref="A26" r:id="rId41"/>
-    <hyperlink ref="C26" r:id="rId42"/>
+    <hyperlink ref="C26" r:id="rId42" display="JSON"/>
     <hyperlink ref="A29" r:id="rId43"/>
-    <hyperlink ref="C29" r:id="rId44"/>
+    <hyperlink ref="C29" r:id="rId44" display="JSON"/>
     <hyperlink ref="A30" r:id="rId45"/>
-    <hyperlink ref="C30" r:id="rId46"/>
+    <hyperlink ref="C30" r:id="rId46" display="JSON"/>
     <hyperlink ref="A31" r:id="rId47"/>
-    <hyperlink ref="C31" r:id="rId48"/>
+    <hyperlink ref="C31" r:id="rId48" display="JSON"/>
     <hyperlink ref="A32" r:id="rId49"/>
-    <hyperlink ref="C32" r:id="rId50"/>
+    <hyperlink ref="C32" r:id="rId50" display="JSON"/>
     <hyperlink ref="A33" r:id="rId51"/>
-    <hyperlink ref="C33" r:id="rId52"/>
+    <hyperlink ref="C33" r:id="rId52" display="JSON"/>
     <hyperlink ref="A34" r:id="rId53"/>
-    <hyperlink ref="C34" r:id="rId54"/>
+    <hyperlink ref="C34" r:id="rId54" display="JSON"/>
     <hyperlink ref="A35" r:id="rId55"/>
-    <hyperlink ref="C35" r:id="rId56"/>
+    <hyperlink ref="C35" r:id="rId56" display="JSON"/>
     <hyperlink ref="A36" r:id="rId57"/>
-    <hyperlink ref="C36" r:id="rId58"/>
+    <hyperlink ref="C36" r:id="rId58" display="JSON"/>
     <hyperlink ref="A37" r:id="rId59"/>
-    <hyperlink ref="C37" r:id="rId60"/>
+    <hyperlink ref="C37" r:id="rId60" display="JSON"/>
     <hyperlink ref="A39" r:id="rId61"/>
-    <hyperlink ref="C39" r:id="rId62"/>
+    <hyperlink ref="C39" r:id="rId62" display="JSON"/>
     <hyperlink ref="A40" r:id="rId63"/>
-    <hyperlink ref="C40" r:id="rId64"/>
+    <hyperlink ref="C40" r:id="rId64" display="JSON"/>
     <hyperlink ref="A41" r:id="rId65"/>
-    <hyperlink ref="C41" r:id="rId66"/>
+    <hyperlink ref="C41" r:id="rId66" display="JSON"/>
     <hyperlink ref="A42" r:id="rId67"/>
-    <hyperlink ref="C42" r:id="rId68"/>
+    <hyperlink ref="C42" r:id="rId68" display="JSON"/>
     <hyperlink ref="A43" r:id="rId69"/>
-    <hyperlink ref="C43" r:id="rId70"/>
+    <hyperlink ref="C43" r:id="rId70" display="JSON"/>
     <hyperlink ref="A44" r:id="rId71"/>
-    <hyperlink ref="C44" r:id="rId72"/>
+    <hyperlink ref="C44" r:id="rId72" display="JSON"/>
     <hyperlink ref="A45" r:id="rId73"/>
-    <hyperlink ref="C45" r:id="rId74"/>
+    <hyperlink ref="C45" r:id="rId74" display="JSON"/>
     <hyperlink ref="A46" r:id="rId75"/>
-    <hyperlink ref="C46" r:id="rId76"/>
+    <hyperlink ref="C46" r:id="rId76" display="JSON"/>
     <hyperlink ref="A47" r:id="rId77"/>
-    <hyperlink ref="C47" r:id="rId78"/>
+    <hyperlink ref="C47" r:id="rId78" display="JSON"/>
     <hyperlink ref="A49" r:id="rId79"/>
-    <hyperlink ref="C49" r:id="rId80"/>
+    <hyperlink ref="C49" r:id="rId80" display="JSON"/>
     <hyperlink ref="A50" r:id="rId81"/>
-    <hyperlink ref="C50" r:id="rId82"/>
+    <hyperlink ref="C50" r:id="rId82" display="JSON"/>
     <hyperlink ref="A51" r:id="rId83"/>
-    <hyperlink ref="C51" r:id="rId84"/>
+    <hyperlink ref="C51" r:id="rId84" display="JSON"/>
     <hyperlink ref="A53" r:id="rId85"/>
-    <hyperlink ref="C53" r:id="rId86"/>
+    <hyperlink ref="C53" r:id="rId86" display="JSON"/>
     <hyperlink ref="A54" r:id="rId87"/>
-    <hyperlink ref="C54" r:id="rId88"/>
+    <hyperlink ref="C54" r:id="rId88" display="JSON"/>
     <hyperlink ref="A55" r:id="rId89"/>
-    <hyperlink ref="C55" r:id="rId90"/>
+    <hyperlink ref="C55" r:id="rId90" display="JSON"/>
     <hyperlink ref="B58" r:id="rId91"/>
-    <hyperlink ref="C58" r:id="rId92"/>
+    <hyperlink ref="C58" r:id="rId92" display="JSON"/>
     <hyperlink ref="A59" r:id="rId93"/>
-    <hyperlink ref="C59" r:id="rId94"/>
+    <hyperlink ref="C59" r:id="rId94" display="JSON"/>
     <hyperlink ref="A60" r:id="rId95"/>
-    <hyperlink ref="C60" r:id="rId96"/>
+    <hyperlink ref="C60" r:id="rId96" display="JSON"/>
     <hyperlink ref="A61" r:id="rId97"/>
-    <hyperlink ref="C61" r:id="rId98"/>
+    <hyperlink ref="C61" r:id="rId98" display="JSON"/>
     <hyperlink ref="A62" r:id="rId99"/>
-    <hyperlink ref="C62" r:id="rId100"/>
+    <hyperlink ref="C62" r:id="rId100" display="JSON"/>
     <hyperlink ref="A56" r:id="rId101"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating Quarterly House Unit Completions (By Type) chart
</commit_message>
<xml_diff>
--- a/docs/DCD_DataSheet.xlsx
+++ b/docs/DCD_DataSheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/losullivan/Documents/repos/bcd-dd-v2.1/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bashir/mydcd/bcd-dd-v2.1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14340" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Landing Page" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="291">
   <si>
     <t>Chart No</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>Annual Water Consumption per Capita</t>
-  </si>
-  <si>
-    <t>Eastern River Basin District Water Quality http://www.epa.ie/</t>
   </si>
   <si>
     <t>1998-2010</t>
@@ -760,13 +757,172 @@
   </si>
   <si>
     <t>https://www.cso.ie/StatbankServices/StatbankServices.svc/jsonservice/responseinstance/ROA27</t>
+  </si>
+  <si>
+    <t>Economy</t>
+  </si>
+  <si>
+    <t>Numbers in Employment</t>
+  </si>
+  <si>
+    <t>https://statbank.cso.ie/px/pxeirestat/Statire/SelectVarVal/Define.asp?maintable=QLF08&amp;PLanguage=0</t>
+  </si>
+  <si>
+    <t>themes#Economy</t>
+  </si>
+  <si>
+    <t>/data/Economy/employment.csv</t>
+  </si>
+  <si>
+    <t>Dublin and the rest of Irekand</t>
+  </si>
+  <si>
+    <t>Numbers Unemployed</t>
+  </si>
+  <si>
+    <t>/data/Economy/QNQ22_2</t>
+  </si>
+  <si>
+    <t>Gross Value Added</t>
+  </si>
+  <si>
+    <t>https://statbank.cso.ie/px/pxeirestat/Statire/SelectVarVal/Define.asp?maintable=raa01</t>
+  </si>
+  <si>
+    <t>/data/Economy/RAA01</t>
+  </si>
+  <si>
+    <t>Dublin , Dublin plus Mid East and State</t>
+  </si>
+  <si>
+    <t>https://statbank.cso.ie/px/pxeirestat/Statire/SelectVarVal/Define.asp?maintable=SIA20&amp;PLanguage=0</t>
+  </si>
+  <si>
+    <t>Poverty Rating</t>
+  </si>
+  <si>
+    <t>/data/Economy/SIA20</t>
+  </si>
+  <si>
+    <t>Dublin  from 2004-2016</t>
+  </si>
+  <si>
+    <t>Numbers by Employment Sector in Dublin</t>
+  </si>
+  <si>
+    <t>https://statbank.cso.ie/px/pxeirestat/Statire/SelectVarVal/Define.asp?maintable=QLF07&amp;PLanguage=0</t>
+  </si>
+  <si>
+    <t>/data/Economy/IncomeAndLivingData</t>
+  </si>
+  <si>
+    <t>/data/Economy/BRA08</t>
+  </si>
+  <si>
+    <t>Dublin from 2008-2016</t>
+  </si>
+  <si>
+    <t>Overseas Visitors</t>
+  </si>
+  <si>
+    <t>http://www.failteireland.ie/Research-Insights/Tourism-Facts-and-Figures.aspx</t>
+  </si>
+  <si>
+    <t>/data/Economy/overseasvisitors</t>
+  </si>
+  <si>
+    <t>Dublin from 2013-2017</t>
+  </si>
+  <si>
+    <t>stacked_area_chart.js</t>
+  </si>
+  <si>
+    <t>multiline_chart.js</t>
+  </si>
+  <si>
+    <t>grouped_bar_chart</t>
+  </si>
+  <si>
+    <t>Median Real Household Disposable Income</t>
+  </si>
+  <si>
+    <t>Number of Employees by Size of Company</t>
+  </si>
+  <si>
+    <t>https://statbank.cso.ie/px/pxeirestat/Statire/SelectVarVal/Define.asp?maintable=BRA08&amp;PLanguage=0</t>
+  </si>
+  <si>
+    <t>/data/Economy/</t>
+  </si>
+  <si>
+    <t>grouped_bar_chart.js</t>
+  </si>
+  <si>
+    <t>stacked_bar_chart.js</t>
+  </si>
+  <si>
+    <t>Eastern River Basin District Water Quality c</t>
+  </si>
+  <si>
+    <t>http://www.epa.ie/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/03/2020 Data Checked from the source and still no update </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/03/2020 Data is upated till </t>
+  </si>
+  <si>
+    <t>Q32019</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> data still the same till Q3 2017</t>
+  </si>
+  <si>
+    <t>Data is updated till 2019 Q4</t>
+  </si>
+  <si>
+    <t>10/03/2020 Data is updated till 2018</t>
+  </si>
+  <si>
+    <t>data still up to 2014</t>
+  </si>
+  <si>
+    <t>data updated to 2018</t>
+  </si>
+  <si>
+    <t>data still not updated till 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> data still not updated till 2016</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>No. of Patients Waiting on Trolleys (30 Weekday Rolling Average)</t>
+  </si>
+  <si>
+    <t>https://www.gov.ie/en/organisation/department-of-health/?referrer=/*</t>
+  </si>
+  <si>
+    <t>theme/Health</t>
+  </si>
+  <si>
+    <t>/data/health/trolleys_transposed.csv</t>
+  </si>
+  <si>
+    <t>Dublin from 2013-2016</t>
+  </si>
+  <si>
+    <t>health.js</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -865,8 +1021,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFB000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFB000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="4"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -909,6 +1118,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -947,7 +1162,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -987,6 +1202,16 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="60% - Accent6" xfId="7" builtinId="52"/>
@@ -1031,6 +1256,11 @@
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFB000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1341,7 +1571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A17:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="B16" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -1359,142 +1589,142 @@
   <sheetData>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="C17" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="D17" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="H17" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="D17" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>100</v>
-      </c>
       <c r="I17" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G18">
         <v>2016</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C20" s="16" t="s">
-        <v>104</v>
-      </c>
       <c r="D20" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="16" t="s">
+      <c r="D21" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>46</v>
-      </c>
       <c r="E21" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="I21" s="16" t="s">
         <v>116</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1515,7 +1745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C28" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -1528,618 +1758,618 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>122</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="20" t="s">
         <v>122</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="23" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2267,46 +2497,46 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2330,10 +2560,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2348,41 +2578,41 @@
     <col min="9" max="9" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -2408,10 +2638,10 @@
         <v>43633</v>
       </c>
       <c r="I3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -2437,10 +2667,18 @@
         <v>43633</v>
       </c>
       <c r="I4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="P4" s="25" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -2466,10 +2704,18 @@
         <v>43633</v>
       </c>
       <c r="I5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="P5" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -2492,15 +2738,26 @@
         <v>43633</v>
       </c>
       <c r="I6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="P6" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>272</v>
+      </c>
+      <c r="C7" t="s">
+        <v>273</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -2509,7 +2766,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>9</v>
@@ -2518,24 +2775,32 @@
         <v>43633</v>
       </c>
       <c r="I7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="P7" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="26"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
         <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>9</v>
@@ -2544,24 +2809,32 @@
         <v>43633</v>
       </c>
       <c r="I8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="P8" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="26"/>
+      <c r="S8" s="26"/>
+      <c r="T8" s="26"/>
+      <c r="U8" s="26"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>9</v>
@@ -2570,366 +2843,750 @@
         <v>43633</v>
       </c>
       <c r="I9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="P9" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="26"/>
+      <c r="T9" s="26"/>
+      <c r="U9" s="26"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="P10" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="26"/>
+      <c r="T10" s="26"/>
+      <c r="U10" s="26"/>
+    </row>
+    <row r="11" spans="1:21" ht="20" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
         <v>30</v>
       </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>31</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>32</v>
       </c>
-      <c r="G12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="P12" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="29" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>2</v>
       </c>
       <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>35</v>
       </c>
-      <c r="F13" t="s">
-        <v>36</v>
-      </c>
       <c r="G13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="P13" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="29"/>
+      <c r="S13" s="29" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>3</v>
       </c>
       <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" t="s">
-        <v>38</v>
-      </c>
       <c r="G14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H14" s="13">
         <v>43633</v>
       </c>
       <c r="I14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="P14" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="29" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>4</v>
       </c>
       <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>42</v>
       </c>
-      <c r="F15" t="s">
-        <v>43</v>
-      </c>
       <c r="G15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H15" s="13">
         <v>43633</v>
       </c>
       <c r="I15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="P15" t="s">
+        <v>275</v>
+      </c>
+      <c r="S15" s="29" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>5</v>
       </c>
       <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" t="s">
         <v>45</v>
       </c>
-      <c r="D16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>46</v>
       </c>
-      <c r="F16" t="s">
-        <v>47</v>
-      </c>
       <c r="G16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+      <c r="P16" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="S16">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>6</v>
       </c>
       <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>49</v>
       </c>
-      <c r="F17" t="s">
-        <v>50</v>
-      </c>
       <c r="G17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H17" s="13">
         <v>43633</v>
       </c>
       <c r="I17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="P17" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>7</v>
       </c>
       <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" t="s">
         <v>57</v>
       </c>
-      <c r="F18" t="s">
-        <v>58</v>
-      </c>
       <c r="G18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H18" s="13">
         <v>43633</v>
       </c>
       <c r="I18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="P18" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>8</v>
       </c>
       <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" t="s">
         <v>54</v>
       </c>
-      <c r="D20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>55</v>
       </c>
-      <c r="F20" t="s">
-        <v>56</v>
-      </c>
       <c r="G20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="P20" s="29" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>9</v>
       </c>
       <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" t="s">
         <v>60</v>
       </c>
-      <c r="D21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>61</v>
-      </c>
-      <c r="F21" t="s">
-        <v>62</v>
       </c>
       <c r="H21" s="13">
         <v>43633</v>
       </c>
       <c r="I21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="P21" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="T21" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>10</v>
       </c>
       <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" t="s">
         <v>64</v>
       </c>
-      <c r="D22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>65</v>
-      </c>
-      <c r="F22" t="s">
-        <v>66</v>
       </c>
       <c r="H22" s="13">
         <v>43633</v>
       </c>
       <c r="I22" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="P22" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="T22" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="20" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H24" s="13">
         <v>43633</v>
       </c>
       <c r="I24" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="P24" s="29" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>2</v>
       </c>
       <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="D25" t="s">
         <v>3</v>
       </c>
       <c r="E25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" t="s">
         <v>74</v>
       </c>
-      <c r="F25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="P25" s="29" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>3</v>
       </c>
       <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="D26" t="s">
         <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="P26" s="29" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F27" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="P27" s="29" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A31" s="23">
+        <v>1</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="O31" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="P31" s="28"/>
+      <c r="Q31" s="28"/>
+      <c r="R31" s="28"/>
+      <c r="S31" s="28"/>
+      <c r="T31" s="28"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A32" s="23">
+        <v>2</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="O32" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="P32" s="28"/>
+      <c r="Q32" s="28"/>
+      <c r="R32" s="28"/>
+      <c r="S32" s="28"/>
+      <c r="T32" s="28"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>246</v>
+      </c>
+      <c r="C33" t="s">
+        <v>247</v>
+      </c>
+      <c r="D33" t="s">
+        <v>241</v>
+      </c>
+      <c r="E33" t="s">
+        <v>248</v>
+      </c>
+      <c r="F33" t="s">
+        <v>249</v>
+      </c>
+      <c r="G33" t="s">
+        <v>264</v>
+      </c>
+      <c r="O33" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="P33" s="28"/>
+      <c r="Q33" s="28"/>
+      <c r="R33" s="28"/>
+      <c r="S33" s="28"/>
+      <c r="T33" s="28"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>266</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="F34" t="s">
+        <v>253</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="O34" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="P34" s="28"/>
+      <c r="Q34" s="28"/>
+      <c r="R34" s="28"/>
+      <c r="S34" s="28"/>
+      <c r="T34" s="28"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>251</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="F35" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="G35" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="O35" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="P35" s="28"/>
+      <c r="Q35" s="28"/>
+      <c r="R35" s="28"/>
+      <c r="S35" s="28"/>
+      <c r="T35" s="28"/>
+    </row>
+    <row r="36" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+      <c r="B36" s="24"/>
+      <c r="O36" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="P36" s="28"/>
+      <c r="Q36" s="28"/>
+      <c r="R36" s="28"/>
+      <c r="S36" s="28"/>
+      <c r="T36" s="28"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>254</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="O37" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="P37" s="28"/>
+      <c r="Q37" s="28"/>
+      <c r="R37" s="28"/>
+      <c r="S37" s="28"/>
+      <c r="T37" s="28"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>267</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="D38" t="s">
+        <v>241</v>
+      </c>
+      <c r="E38" t="s">
+        <v>269</v>
+      </c>
+      <c r="F38" t="s">
+        <v>258</v>
+      </c>
+      <c r="G38" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>259</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>261</v>
+      </c>
+      <c r="F39" t="s">
+        <v>262</v>
+      </c>
+      <c r="G39" s="22" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" ht="24" x14ac:dyDescent="0.3">
+      <c r="A41" s="30" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>285</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="D42" t="s">
+        <v>287</v>
+      </c>
+      <c r="E42" t="s">
+        <v>288</v>
+      </c>
+      <c r="F42" t="s">
+        <v>289</v>
+      </c>
+      <c r="G42" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating charts and DCD_Datasheet
</commit_message>
<xml_diff>
--- a/docs/DCD_DataSheet.xlsx
+++ b/docs/DCD_DataSheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/losullivan/Documents/repos/bcd-dd-v2.1/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bashir/nrepo10/bcd-dd-v2.1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19420" activeTab="3"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="27280" windowHeight="14480" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Landing Page" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="293">
   <si>
     <t>Chart No</t>
   </si>
@@ -916,13 +916,19 @@
   </si>
   <si>
     <t>data still the same till Q3 2017</t>
+  </si>
+  <si>
+    <t>Chart was updated in 20/03/2020</t>
+  </si>
+  <si>
+    <t>Chart was updated in 2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1081,6 +1087,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -1175,7 +1195,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1234,6 +1254,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="10" borderId="0" xfId="11"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="60% - Accent6" xfId="7" builtinId="52"/>
@@ -1281,6 +1303,7 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FF59F700"/>
       <color rgb="FFFFB000"/>
     </mruColors>
   </colors>
@@ -2585,8 +2608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2600,6 +2623,7 @@
     <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.83203125" style="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="48.1640625" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20" x14ac:dyDescent="0.2">
@@ -3085,6 +3109,9 @@
       <c r="J17" s="28" t="s">
         <v>290</v>
       </c>
+      <c r="K17" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
@@ -3117,6 +3144,9 @@
       <c r="J18" s="28" t="s">
         <v>275</v>
       </c>
+      <c r="K18" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -3142,6 +3172,12 @@
       </c>
       <c r="J20" s="28" t="s">
         <v>276</v>
+      </c>
+      <c r="K20" t="s">
+        <v>292</v>
+      </c>
+      <c r="M20" s="13">
+        <v>43910</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -3347,9 +3383,11 @@
       <c r="J31" s="26" t="s">
         <v>274</v>
       </c>
-      <c r="K31" s="27"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="27"/>
+      <c r="K31" s="34" t="s">
+        <v>291</v>
+      </c>
+      <c r="L31" s="34"/>
+      <c r="M31" s="34"/>
       <c r="N31" s="27"/>
       <c r="O31" s="27"/>
     </row>
@@ -3380,9 +3418,11 @@
       <c r="J32" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="K32" s="27"/>
-      <c r="L32" s="27"/>
-      <c r="M32" s="27"/>
+      <c r="K32" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="L32" s="35"/>
+      <c r="M32" s="35"/>
       <c r="N32" s="27"/>
       <c r="O32" s="27"/>
     </row>

</xml_diff>

<commit_message>
Amend data source list
</commit_message>
<xml_diff>
--- a/docs/DCD_DataSheet.xlsx
+++ b/docs/DCD_DataSheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28615"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bashir/nrepo10/bcd-dd-v2.1/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/losullivan/Documents/repos/bcd-dd-v2.1/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="27280" windowHeight="14480" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22420" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Landing Page" sheetId="2" r:id="rId1"/>
@@ -38,8 +38,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="E31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+LOS- Switch to use statbank </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="288">
   <si>
     <t>Chart No</t>
   </si>
@@ -834,15 +866,6 @@
     <t>Dublin from 2013-2017</t>
   </si>
   <si>
-    <t>stacked_area_chart.js</t>
-  </si>
-  <si>
-    <t>multiline_chart.js</t>
-  </si>
-  <si>
-    <t>grouped_bar_chart</t>
-  </si>
-  <si>
     <t>Median Real Household Disposable Income</t>
   </si>
   <si>
@@ -853,12 +876,6 @@
   </si>
   <si>
     <t>/data/Economy/</t>
-  </si>
-  <si>
-    <t>grouped_bar_chart.js</t>
-  </si>
-  <si>
-    <t>stacked_bar_chart.js</t>
   </si>
   <si>
     <t>Eastern River Basin District Water Quality c</t>
@@ -928,7 +945,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1100,6 +1117,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1618,7 +1646,7 @@
   <dimension ref="A17:I22"/>
   <sheetViews>
     <sheetView topLeftCell="B16" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1791,9 +1819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C28" sqref="C1:C1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2605,11 +2631,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D4" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2660,10 +2686,10 @@
         <v>86</v>
       </c>
       <c r="J2" s="33" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="K2" s="33" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="165" x14ac:dyDescent="0.2">
@@ -2724,7 +2750,7 @@
         <v>90</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
@@ -2761,7 +2787,7 @@
         <v>90</v>
       </c>
       <c r="J5" s="25" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="K5" s="25"/>
       <c r="L5" s="25"/>
@@ -2795,7 +2821,7 @@
         <v>87</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="K6" s="25"/>
       <c r="L6" s="25"/>
@@ -2808,10 +2834,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -2832,7 +2858,7 @@
         <v>87</v>
       </c>
       <c r="J7" s="25" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
@@ -2866,7 +2892,7 @@
         <v>87</v>
       </c>
       <c r="J8" s="25" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
@@ -2900,7 +2926,7 @@
         <v>87</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="K9" s="25"/>
       <c r="L9" s="25"/>
@@ -2910,7 +2936,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="J10" s="25" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="K10" s="25"/>
       <c r="L10" s="25"/>
@@ -2946,7 +2972,7 @@
         <v>32</v>
       </c>
       <c r="J12" s="28" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="K12" s="28"/>
       <c r="L12" s="28"/>
@@ -2975,7 +3001,7 @@
         <v>32</v>
       </c>
       <c r="J13" s="28" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="K13" s="28"/>
       <c r="L13" s="28"/>
@@ -3010,7 +3036,7 @@
         <v>87</v>
       </c>
       <c r="J14" s="28" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="K14" s="28"/>
       <c r="L14" s="28"/>
@@ -3045,7 +3071,7 @@
         <v>87</v>
       </c>
       <c r="J15" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="M15" s="28"/>
     </row>
@@ -3075,7 +3101,7 @@
         <v>91</v>
       </c>
       <c r="J16" s="28" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -3107,10 +3133,10 @@
         <v>87</v>
       </c>
       <c r="J17" s="28" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="K17" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -3142,10 +3168,10 @@
         <v>87</v>
       </c>
       <c r="J18" s="28" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="K18" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -3171,10 +3197,10 @@
         <v>32</v>
       </c>
       <c r="J20" s="28" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="K20" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="M20" s="13">
         <v>43910</v>
@@ -3206,7 +3232,7 @@
         <v>87</v>
       </c>
       <c r="J21" s="28" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
@@ -3235,7 +3261,7 @@
         <v>87</v>
       </c>
       <c r="J22" s="28" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="20" x14ac:dyDescent="0.2">
@@ -3269,7 +3295,7 @@
         <v>87</v>
       </c>
       <c r="J24" s="28" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
@@ -3292,7 +3318,7 @@
         <v>74</v>
       </c>
       <c r="J25" s="28" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -3315,7 +3341,7 @@
         <v>69</v>
       </c>
       <c r="J26" s="28" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
@@ -3338,7 +3364,7 @@
         <v>80</v>
       </c>
       <c r="J27" s="28" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -3375,16 +3401,14 @@
       <c r="F31" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="G31" s="21" t="s">
-        <v>263</v>
-      </c>
+      <c r="G31" s="21"/>
       <c r="H31" s="21"/>
       <c r="I31" s="32"/>
       <c r="J31" s="26" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="K31" s="34" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="L31" s="34"/>
       <c r="M31" s="34"/>
@@ -3410,16 +3434,14 @@
       <c r="F32" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="G32" s="21" t="s">
-        <v>263</v>
-      </c>
+      <c r="G32" s="21"/>
       <c r="H32" s="21"/>
       <c r="I32" s="32"/>
       <c r="J32" s="27" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="K32" s="35" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="L32" s="35"/>
       <c r="M32" s="35"/>
@@ -3445,11 +3467,8 @@
       <c r="F33" t="s">
         <v>249</v>
       </c>
-      <c r="G33" t="s">
-        <v>264</v>
-      </c>
       <c r="J33" s="27" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="K33" s="27"/>
       <c r="L33" s="27"/>
@@ -3462,7 +3481,7 @@
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C34" s="21" t="s">
         <v>250</v>
@@ -3476,11 +3495,9 @@
       <c r="F34" t="s">
         <v>253</v>
       </c>
-      <c r="G34" s="21" t="s">
-        <v>265</v>
-      </c>
+      <c r="G34" s="21"/>
       <c r="J34" s="27" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="K34" s="27"/>
       <c r="L34" s="27"/>
@@ -3507,11 +3524,9 @@
       <c r="F35" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="G35" s="21" t="s">
-        <v>271</v>
-      </c>
+      <c r="G35" s="21"/>
       <c r="J35" s="27" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="K35" s="27"/>
       <c r="L35" s="27"/>
@@ -3522,7 +3537,7 @@
     <row r="36" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="B36" s="23"/>
       <c r="J36" s="27" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="K36" s="27"/>
       <c r="L36" s="27"/>
@@ -3550,7 +3565,7 @@
         <v>258</v>
       </c>
       <c r="J37" s="27" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="K37" s="27"/>
       <c r="L37" s="27"/>
@@ -3563,22 +3578,19 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D38" t="s">
         <v>241</v>
       </c>
       <c r="E38" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F38" t="s">
         <v>258</v>
-      </c>
-      <c r="G38" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
@@ -3600,13 +3612,11 @@
       <c r="F39" t="s">
         <v>262</v>
       </c>
-      <c r="G39" s="21" t="s">
-        <v>270</v>
-      </c>
+      <c r="G39" s="21"/>
     </row>
     <row r="41" spans="1:15" ht="24" x14ac:dyDescent="0.3">
       <c r="A41" s="29" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
@@ -3614,22 +3624,22 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
+        <v>275</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="D42" t="s">
+        <v>277</v>
+      </c>
+      <c r="E42" t="s">
+        <v>278</v>
+      </c>
+      <c r="F42" t="s">
+        <v>279</v>
+      </c>
+      <c r="G42" t="s">
         <v>280</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>281</v>
-      </c>
-      <c r="D42" t="s">
-        <v>282</v>
-      </c>
-      <c r="E42" t="s">
-        <v>283</v>
-      </c>
-      <c r="F42" t="s">
-        <v>284</v>
-      </c>
-      <c r="G42" t="s">
-        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -3656,5 +3666,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
+  <legacyDrawing r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add housing story data to DCD_DataSheet
Added a new tab with data used in housing story phases 1, 2, 3

Biggest outstanding problems involve finding sources for most of the housing data

Much of the data is simliar to data in the Themes tab, but reformatted or different timeframes. Some reconciling may be necessary.

Decide which of the story data also belongs as a new Themes chart?
</commit_message>
<xml_diff>
--- a/docs/DCD_DataSheet.xlsx
+++ b/docs/DCD_DataSheet.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22904"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/losullivan/Documents/repos/bcd-dd-v2.1/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sstehle\BCD\Dashboard_sandbox\bcd-dd-v2.1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1C7B6CD-451F-4FA9-9838-808A092CF77E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22420" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8205" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Landing Page" sheetId="2" r:id="rId1"/>
     <sheet name="Statbank" sheetId="3" r:id="rId2"/>
     <sheet name="discontinued_politcal football" sheetId="4" r:id="rId3"/>
     <sheet name="Themes Page" sheetId="1" r:id="rId4"/>
+    <sheet name="Stories" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191028" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,12 +42,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="E39" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="E40" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="409">
   <si>
     <t>Card</t>
   </si>
@@ -1017,13 +1017,301 @@
   </si>
   <si>
     <t>Some health variable???</t>
+  </si>
+  <si>
+    <t>http://insideairbnb.com/get-the-data.html</t>
+  </si>
+  <si>
+    <t>https://data-housinggovie.opendata.arcgis.com/datasets</t>
+  </si>
+  <si>
+    <t>data current as of Q3 2019 - archive back to Q4 2017 to be downloaded</t>
+  </si>
+  <si>
+    <t>/stories#phase_3</t>
+  </si>
+  <si>
+    <t>Rent prices jumped, particularly in Dublin</t>
+  </si>
+  <si>
+    <t>All counties + whole state minus Dublin, Q4 2007-Q1 2019</t>
+  </si>
+  <si>
+    <t>story-housing3-fig1.js</t>
+  </si>
+  <si>
+    <t>data is different from above</t>
+  </si>
+  <si>
+    <t>what is source?</t>
+  </si>
+  <si>
+    <t>New and second-hand home prices rose dramatically</t>
+  </si>
+  <si>
+    <t>/stories#phase_1</t>
+  </si>
+  <si>
+    <t>story-housing1-fig4.js</t>
+  </si>
+  <si>
+    <t>/themes#housing, /storiesphase_2</t>
+  </si>
+  <si>
+    <t>Housing unit completions outnumbered new households</t>
+  </si>
+  <si>
+    <t>story-housing1-fig3.js</t>
+  </si>
+  <si>
+    <t>story-housing3-fig4.js</t>
+  </si>
+  <si>
+    <t>how to auto update with new data?</t>
+  </si>
+  <si>
+    <t>add to themes page</t>
+  </si>
+  <si>
+    <t>monthly updates in individual geojson - this is the most recent from Mar 2020</t>
+  </si>
+  <si>
+    <t>story-housing3-fig3.js</t>
+  </si>
+  <si>
+    <t>monthly updates, processed in R for plotly</t>
+  </si>
+  <si>
+    <t>story-housing3-fig5.js</t>
+  </si>
+  <si>
+    <t>Dublin Housing Task Force quarterly updates of Tier 1 and Tier 2A housing development proposals from Q4 2019</t>
+  </si>
+  <si>
+    <t>phase 1</t>
+  </si>
+  <si>
+    <t>phase 2</t>
+  </si>
+  <si>
+    <t>phase 3</t>
+  </si>
+  <si>
+    <t>Population and households surged from 1991 - 2006, increasing housing demand</t>
+  </si>
+  <si>
+    <t>Dublin area housing type diversity also increased</t>
+  </si>
+  <si>
+    <t>Cost versus wage discrepancy increased mortgage debt</t>
+  </si>
+  <si>
+    <t>Demand for social housing and long-term rentals increased</t>
+  </si>
+  <si>
+    <t>High prices led to more renting, less social housing</t>
+  </si>
+  <si>
+    <t>Urban prices drove sprawl and long-distance commuting</t>
+  </si>
+  <si>
+    <t>After rapid growth, property prices collapsed</t>
+  </si>
+  <si>
+    <t>More homes were being built than demanded, leading to high vacancy rates</t>
+  </si>
+  <si>
+    <t>Estates remained unfinished throughout the country</t>
+  </si>
+  <si>
+    <t>Non-residential properties were also left vacant</t>
+  </si>
+  <si>
+    <t>High mortgage rates meant many could not afford payments</t>
+  </si>
+  <si>
+    <t>Buy-to-rent mortgages experienced higher rates of arrears</t>
+  </si>
+  <si>
+    <t>High housing costs drove many more to seek social housing</t>
+  </si>
+  <si>
+    <t>Housing assistance for Traveller families also declined</t>
+  </si>
+  <si>
+    <t>High rents and comparatively low wages drove homelessness rates higher</t>
+  </si>
+  <si>
+    <t>The short term rental market displaces housing stock for residents</t>
+  </si>
+  <si>
+    <t>Regulations have not curbed the short-term rental problem</t>
+  </si>
+  <si>
+    <t>Development continues to expand, especially in higher income areas</t>
+  </si>
+  <si>
+    <t>/stories#phase_2</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_1/pop_house.csv</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_1/housetype.csv</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_1/housecomp.csv</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_1/propertyprices.csv</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_1/mortgage_debt.csv</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_1/House_Com.csv</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_1/Social_housing_stock.csv</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_1/DublinCityDestPOWCAR11_0.js</t>
+  </si>
+  <si>
+    <t>story-housing1-fig1.js</t>
+  </si>
+  <si>
+    <t>story-housing1-fig2.js</t>
+  </si>
+  <si>
+    <t>story-housing1-fig5.js</t>
+  </si>
+  <si>
+    <t>story-housing1-fig6.js</t>
+  </si>
+  <si>
+    <t>story-housing1-fig7.js</t>
+  </si>
+  <si>
+    <t>story-housing1-fig9.js</t>
+  </si>
+  <si>
+    <t>yearly average of "monthly housing unit completions" in Themes data with longer range</t>
+  </si>
+  <si>
+    <t>data is a yearly version of the quarterly "average house prices" data in the Themes page, but is not an average</t>
+  </si>
+  <si>
+    <t>county level breakdown of "population statistics" data on Themes page</t>
+  </si>
+  <si>
+    <t>census year breakdown of house types</t>
+  </si>
+  <si>
+    <t>yearly 2002 - 2007</t>
+  </si>
+  <si>
+    <t>social housing units by LA 1994 - 2016</t>
+  </si>
+  <si>
+    <t>census year breakdown of house tenure by LA</t>
+  </si>
+  <si>
+    <t>POWSCAR subset to only include Eds with # commuters to Dublin City</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_2/processed/E1071.csv</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_2/processed/unifinished_estates_2010_bnsd_dublin_area.csv</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_2/processed/serviced_land_hectares.csv, /data/Stories/Housing/part_2/processed/serviced_land_expected_units.csv</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_2/processed/home_mortgage_arrears.csv</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_2/processed/btl_mortgage_arrears.csv</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_2/processed/social_housing_wait_list.csv</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_2/processed/traveller_accomodation_accomodated.csv</t>
+  </si>
+  <si>
+    <t>story-housing2-fig1.js</t>
+  </si>
+  <si>
+    <t>story-housing2-fig2.js</t>
+  </si>
+  <si>
+    <t>story-housing2-fig3.js</t>
+  </si>
+  <si>
+    <t>story-housing2-fig4.js</t>
+  </si>
+  <si>
+    <t>story-housing2-fig5.js</t>
+  </si>
+  <si>
+    <t>story-housing2-fig6.js</t>
+  </si>
+  <si>
+    <t>story-housing2-fig7.js</t>
+  </si>
+  <si>
+    <t>story-housing2-fig8.js</t>
+  </si>
+  <si>
+    <t>monthly property price index Dublin, rest of Ireland, and national. Monthly 2005-2019 Jan</t>
+  </si>
+  <si>
+    <t>census year numbers of vacant units and % vacant</t>
+  </si>
+  <si>
+    <t>map of unfinshed estates 2010</t>
+  </si>
+  <si>
+    <t>vacant serviced zoned land yearly 2000 - 2012 for 4 LAs and surrounding counties</t>
+  </si>
+  <si>
+    <t>accounts in mortgage arrears monthly Sept 2009 - Dec 2017</t>
+  </si>
+  <si>
+    <t>buy to rent mortgage arrears tri-monthly Jun 2012 - Jun 2018</t>
+  </si>
+  <si>
+    <t>people in social housing nationally every tree years 1991 - 2018</t>
+  </si>
+  <si>
+    <t>unauthorised and accommodated Traveller sites nationally and 4 LAs yearly 2002-2013</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_3/processed/ave_monthly_rent.csv</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_3/processed/homeless_figures_parsed.csv, /data/Stories/Housing/part_3/processed/drhe_homelessness.csv</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_3/processed/Airbnb_listings_Mar2020.csv</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_3/processed/airbnb_counts.csv</t>
+  </si>
+  <si>
+    <t>/data/Stories/Housing/part_3/Dublin_Housing_Task_Force_Q3_2019_T1.geojson, /data/Stories/Housing/part_3/Dublin_Housing_Task_Force_Q3_2019_T2A.geojson</t>
+  </si>
+  <si>
+    <t>individuals and families monthly nationally, June 2014 - Nov 2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="32">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1240,8 +1528,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1325,6 +1619,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1364,7 +1664,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -1470,6 +1770,27 @@
     <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="8" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="60% - Accent6" xfId="7" builtinId="52"/>
@@ -1510,7 +1831,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1828,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A17:I22"/>
   <sheetViews>
     <sheetView topLeftCell="B16" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
@@ -1958,7 +2279,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30">
+    <row r="21" spans="1:9" ht="45">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -2002,7 +2323,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2022,7 +2343,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="23.1">
+    <row r="2" spans="1:3" ht="21.75">
       <c r="A2" s="17" t="s">
         <v>36</v>
       </c>
@@ -2071,7 +2392,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="23.1">
+    <row r="7" spans="1:3" ht="21.75">
       <c r="A7" s="17" t="s">
         <v>46</v>
       </c>
@@ -2109,7 +2430,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="23.1">
+    <row r="11" spans="1:3" ht="21.75">
       <c r="A11" s="17" t="s">
         <v>53</v>
       </c>
@@ -2224,7 +2545,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="23.1">
+    <row r="22" spans="1:3" ht="21.75">
       <c r="A22" s="17" t="s">
         <v>74</v>
       </c>
@@ -2273,7 +2594,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="23.1">
+    <row r="27" spans="1:3" ht="21.75">
       <c r="A27" s="17" t="s">
         <v>83</v>
       </c>
@@ -2385,7 +2706,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="23.1">
+    <row r="38" spans="1:3" ht="21.75">
       <c r="A38" s="17" t="s">
         <v>102</v>
       </c>
@@ -2489,7 +2810,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="23.1">
+    <row r="48" spans="1:3" ht="21.75">
       <c r="A48" s="17" t="s">
         <v>121</v>
       </c>
@@ -2527,7 +2848,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="23.1">
+    <row r="52" spans="1:3" ht="21.75">
       <c r="A52" s="17" t="s">
         <v>128</v>
       </c>
@@ -2570,7 +2891,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="23.1">
+    <row r="57" spans="1:3" ht="21.75">
       <c r="A57" s="17" t="s">
         <v>136</v>
       </c>
@@ -2633,107 +2954,107 @@
   </sheetData>
   <dataConsolidate/>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" display="JSON" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="C4" r:id="rId4" display="JSON" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="A5" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="C5" r:id="rId6" display="JSON" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="A6" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="C6" r:id="rId8" display="JSON" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="A8" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="C8" r:id="rId10" display="JSON" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="A10" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="C10" r:id="rId12" display="JSON" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="A9" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="C9" r:id="rId14" display="JSON" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="A12" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="C12" r:id="rId16" display="JSON" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="A13" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="C13" r:id="rId18" display="JSON" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="A14" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="C14" r:id="rId20" display="JSON" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="A15" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="C15" r:id="rId22" display="JSON" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="A16" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="C16" r:id="rId24" display="JSON" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="A17" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="C17" r:id="rId26" display="JSON" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="A18" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="C18" r:id="rId28" display="JSON" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="A19" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="C19" r:id="rId30" display="JSON" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="A20" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="C20" r:id="rId32" display="JSON" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="A21" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="C21" r:id="rId34" display="JSON" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="A23" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="C23" r:id="rId36" display="JSON" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="A24" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="C24" r:id="rId38" display="JSON" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
-    <hyperlink ref="A25" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="C25" r:id="rId40" display="JSON" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
-    <hyperlink ref="A26" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="C26" r:id="rId42" display="JSON" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
-    <hyperlink ref="A29" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="C29" r:id="rId44" display="JSON" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="A30" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="C30" r:id="rId46" display="JSON" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="A31" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="C31" r:id="rId48" display="JSON" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="A32" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="C32" r:id="rId50" display="JSON" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink ref="A33" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
-    <hyperlink ref="C33" r:id="rId52" display="JSON" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
-    <hyperlink ref="A34" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
-    <hyperlink ref="C34" r:id="rId54" display="JSON" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
-    <hyperlink ref="A35" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
-    <hyperlink ref="C35" r:id="rId56" display="JSON" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
-    <hyperlink ref="A36" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
-    <hyperlink ref="C36" r:id="rId58" display="JSON" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
-    <hyperlink ref="A37" r:id="rId59" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
-    <hyperlink ref="C37" r:id="rId60" display="JSON" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
-    <hyperlink ref="A39" r:id="rId61" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
-    <hyperlink ref="C39" r:id="rId62" display="JSON" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
-    <hyperlink ref="A40" r:id="rId63" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
-    <hyperlink ref="C40" r:id="rId64" display="JSON" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
-    <hyperlink ref="A41" r:id="rId65" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
-    <hyperlink ref="C41" r:id="rId66" display="JSON" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
-    <hyperlink ref="A42" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
-    <hyperlink ref="C42" r:id="rId68" display="JSON" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
-    <hyperlink ref="A43" r:id="rId69" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
-    <hyperlink ref="C43" r:id="rId70" display="JSON" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
-    <hyperlink ref="A44" r:id="rId71" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
-    <hyperlink ref="C44" r:id="rId72" display="JSON" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
-    <hyperlink ref="A45" r:id="rId73" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
-    <hyperlink ref="C45" r:id="rId74" display="JSON" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
-    <hyperlink ref="A46" r:id="rId75" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
-    <hyperlink ref="C46" r:id="rId76" display="JSON" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
-    <hyperlink ref="A47" r:id="rId77" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
-    <hyperlink ref="C47" r:id="rId78" display="JSON" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
-    <hyperlink ref="A49" r:id="rId79" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
-    <hyperlink ref="C49" r:id="rId80" display="JSON" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
-    <hyperlink ref="A50" r:id="rId81" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
-    <hyperlink ref="C50" r:id="rId82" display="JSON" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
-    <hyperlink ref="A51" r:id="rId83" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
-    <hyperlink ref="C51" r:id="rId84" display="JSON" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
-    <hyperlink ref="A53" r:id="rId85" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
-    <hyperlink ref="C53" r:id="rId86" display="JSON" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
-    <hyperlink ref="A54" r:id="rId87" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
-    <hyperlink ref="C54" r:id="rId88" display="JSON" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
-    <hyperlink ref="A55" r:id="rId89" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
-    <hyperlink ref="C55" r:id="rId90" display="JSON" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
-    <hyperlink ref="B58" r:id="rId91" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
-    <hyperlink ref="C58" r:id="rId92" display="JSON" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
-    <hyperlink ref="A59" r:id="rId93" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
-    <hyperlink ref="C59" r:id="rId94" display="JSON" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
-    <hyperlink ref="A60" r:id="rId95" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
-    <hyperlink ref="C60" r:id="rId96" display="JSON" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
-    <hyperlink ref="A61" r:id="rId97" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
-    <hyperlink ref="C61" r:id="rId98" display="JSON" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
-    <hyperlink ref="A62" r:id="rId99" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
-    <hyperlink ref="C62" r:id="rId100" display="JSON" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
-    <hyperlink ref="A56" r:id="rId101" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2" display="JSON"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId4" display="JSON"/>
+    <hyperlink ref="A5" r:id="rId5"/>
+    <hyperlink ref="C5" r:id="rId6" display="JSON"/>
+    <hyperlink ref="A6" r:id="rId7"/>
+    <hyperlink ref="C6" r:id="rId8" display="JSON"/>
+    <hyperlink ref="A8" r:id="rId9"/>
+    <hyperlink ref="C8" r:id="rId10" display="JSON"/>
+    <hyperlink ref="A10" r:id="rId11"/>
+    <hyperlink ref="C10" r:id="rId12" display="JSON"/>
+    <hyperlink ref="A9" r:id="rId13"/>
+    <hyperlink ref="C9" r:id="rId14" display="JSON"/>
+    <hyperlink ref="A12" r:id="rId15"/>
+    <hyperlink ref="C12" r:id="rId16" display="JSON"/>
+    <hyperlink ref="A13" r:id="rId17"/>
+    <hyperlink ref="C13" r:id="rId18" display="JSON"/>
+    <hyperlink ref="A14" r:id="rId19"/>
+    <hyperlink ref="C14" r:id="rId20" display="JSON"/>
+    <hyperlink ref="A15" r:id="rId21"/>
+    <hyperlink ref="C15" r:id="rId22" display="JSON"/>
+    <hyperlink ref="A16" r:id="rId23"/>
+    <hyperlink ref="C16" r:id="rId24" display="JSON"/>
+    <hyperlink ref="A17" r:id="rId25"/>
+    <hyperlink ref="C17" r:id="rId26" display="JSON"/>
+    <hyperlink ref="A18" r:id="rId27"/>
+    <hyperlink ref="C18" r:id="rId28" display="JSON"/>
+    <hyperlink ref="A19" r:id="rId29"/>
+    <hyperlink ref="C19" r:id="rId30" display="JSON"/>
+    <hyperlink ref="A20" r:id="rId31"/>
+    <hyperlink ref="C20" r:id="rId32" display="JSON"/>
+    <hyperlink ref="A21" r:id="rId33"/>
+    <hyperlink ref="C21" r:id="rId34" display="JSON"/>
+    <hyperlink ref="A23" r:id="rId35"/>
+    <hyperlink ref="C23" r:id="rId36" display="JSON"/>
+    <hyperlink ref="A24" r:id="rId37"/>
+    <hyperlink ref="C24" r:id="rId38" display="JSON"/>
+    <hyperlink ref="A25" r:id="rId39"/>
+    <hyperlink ref="C25" r:id="rId40" display="JSON"/>
+    <hyperlink ref="A26" r:id="rId41"/>
+    <hyperlink ref="C26" r:id="rId42" display="JSON"/>
+    <hyperlink ref="A29" r:id="rId43"/>
+    <hyperlink ref="C29" r:id="rId44" display="JSON"/>
+    <hyperlink ref="A30" r:id="rId45"/>
+    <hyperlink ref="C30" r:id="rId46" display="JSON"/>
+    <hyperlink ref="A31" r:id="rId47"/>
+    <hyperlink ref="C31" r:id="rId48" display="JSON"/>
+    <hyperlink ref="A32" r:id="rId49"/>
+    <hyperlink ref="C32" r:id="rId50" display="JSON"/>
+    <hyperlink ref="A33" r:id="rId51"/>
+    <hyperlink ref="C33" r:id="rId52" display="JSON"/>
+    <hyperlink ref="A34" r:id="rId53"/>
+    <hyperlink ref="C34" r:id="rId54" display="JSON"/>
+    <hyperlink ref="A35" r:id="rId55"/>
+    <hyperlink ref="C35" r:id="rId56" display="JSON"/>
+    <hyperlink ref="A36" r:id="rId57"/>
+    <hyperlink ref="C36" r:id="rId58" display="JSON"/>
+    <hyperlink ref="A37" r:id="rId59"/>
+    <hyperlink ref="C37" r:id="rId60" display="JSON"/>
+    <hyperlink ref="A39" r:id="rId61"/>
+    <hyperlink ref="C39" r:id="rId62" display="JSON"/>
+    <hyperlink ref="A40" r:id="rId63"/>
+    <hyperlink ref="C40" r:id="rId64" display="JSON"/>
+    <hyperlink ref="A41" r:id="rId65"/>
+    <hyperlink ref="C41" r:id="rId66" display="JSON"/>
+    <hyperlink ref="A42" r:id="rId67"/>
+    <hyperlink ref="C42" r:id="rId68" display="JSON"/>
+    <hyperlink ref="A43" r:id="rId69"/>
+    <hyperlink ref="C43" r:id="rId70" display="JSON"/>
+    <hyperlink ref="A44" r:id="rId71"/>
+    <hyperlink ref="C44" r:id="rId72" display="JSON"/>
+    <hyperlink ref="A45" r:id="rId73"/>
+    <hyperlink ref="C45" r:id="rId74" display="JSON"/>
+    <hyperlink ref="A46" r:id="rId75"/>
+    <hyperlink ref="C46" r:id="rId76" display="JSON"/>
+    <hyperlink ref="A47" r:id="rId77"/>
+    <hyperlink ref="C47" r:id="rId78" display="JSON"/>
+    <hyperlink ref="A49" r:id="rId79"/>
+    <hyperlink ref="C49" r:id="rId80" display="JSON"/>
+    <hyperlink ref="A50" r:id="rId81"/>
+    <hyperlink ref="C50" r:id="rId82" display="JSON"/>
+    <hyperlink ref="A51" r:id="rId83"/>
+    <hyperlink ref="C51" r:id="rId84" display="JSON"/>
+    <hyperlink ref="A53" r:id="rId85"/>
+    <hyperlink ref="C53" r:id="rId86" display="JSON"/>
+    <hyperlink ref="A54" r:id="rId87"/>
+    <hyperlink ref="C54" r:id="rId88" display="JSON"/>
+    <hyperlink ref="A55" r:id="rId89"/>
+    <hyperlink ref="C55" r:id="rId90" display="JSON"/>
+    <hyperlink ref="B58" r:id="rId91"/>
+    <hyperlink ref="C58" r:id="rId92" display="JSON"/>
+    <hyperlink ref="A59" r:id="rId93"/>
+    <hyperlink ref="C59" r:id="rId94" display="JSON"/>
+    <hyperlink ref="A60" r:id="rId95"/>
+    <hyperlink ref="C60" r:id="rId96" display="JSON"/>
+    <hyperlink ref="A61" r:id="rId97"/>
+    <hyperlink ref="C61" r:id="rId98" display="JSON"/>
+    <hyperlink ref="A62" r:id="rId99"/>
+    <hyperlink ref="C62" r:id="rId100" display="JSON"/>
+    <hyperlink ref="A56" r:id="rId101"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2741,7 +3062,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2799,29 +3120,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="B4" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="C4" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="A5" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="B5" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="C5" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
-    <hyperlink ref="A6" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
-    <hyperlink ref="B6" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
-    <hyperlink ref="C6" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="C4" r:id="rId6"/>
+    <hyperlink ref="A5" r:id="rId7"/>
+    <hyperlink ref="B5" r:id="rId8"/>
+    <hyperlink ref="C5" r:id="rId9"/>
+    <hyperlink ref="A6" r:id="rId10"/>
+    <hyperlink ref="B6" r:id="rId11"/>
+    <hyperlink ref="C6" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:O52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52:K52"/>
+    <sheetView topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2880,7 +3201,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="60">
+    <row r="3" spans="1:15" ht="61.5">
       <c r="A3" s="32"/>
       <c r="B3" s="33" t="s">
         <v>164</v>
@@ -3391,7 +3712,7 @@
         <v>229</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>216</v>
+        <v>325</v>
       </c>
       <c r="E23" s="33" t="s">
         <v>25</v>
@@ -3617,68 +3938,45 @@
       </c>
       <c r="K30" s="43"/>
     </row>
-    <row r="31" spans="1:15" ht="20.25">
-      <c r="A31" s="5" t="s">
+    <row r="31" spans="1:15" s="79" customFormat="1">
+      <c r="C31" s="80"/>
+      <c r="H31" s="81"/>
+      <c r="I31" s="82"/>
+      <c r="J31" s="83"/>
+    </row>
+    <row r="32" spans="1:15" ht="20.25">
+      <c r="A32" s="5" t="s">
         <v>259</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15">
-      <c r="A32" s="40">
-        <v>1</v>
-      </c>
-      <c r="B32" s="33" t="s">
-        <v>260</v>
-      </c>
-      <c r="C32" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="41" t="s">
-        <v>261</v>
-      </c>
-      <c r="E32" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="33" t="s">
-        <v>262</v>
-      </c>
-      <c r="G32" s="33"/>
-      <c r="H32" s="42">
-        <v>43633</v>
-      </c>
-      <c r="I32" s="34" t="s">
-        <v>198</v>
-      </c>
-      <c r="J32" s="52" t="s">
-        <v>263</v>
-      </c>
-      <c r="K32" s="53" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C33" s="41" t="s">
-        <v>265</v>
-      </c>
-      <c r="D33" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="41" t="s">
         <v>261</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>266</v>
+        <v>12</v>
       </c>
       <c r="F33" s="33" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="34"/>
+      <c r="H33" s="42">
+        <v>43633</v>
+      </c>
+      <c r="I33" s="34" t="s">
+        <v>198</v>
+      </c>
       <c r="J33" s="52" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="K33" s="53" t="s">
         <v>221</v>
@@ -3686,28 +3984,28 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C34" s="41" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D34" s="33" t="s">
         <v>261</v>
       </c>
       <c r="E34" s="33" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F34" s="33" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="G34" s="33"/>
       <c r="H34" s="33"/>
       <c r="I34" s="34"/>
       <c r="J34" s="52" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="K34" s="53" t="s">
         <v>221</v>
@@ -3715,22 +4013,22 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C35" s="41" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="D35" s="33" t="s">
         <v>261</v>
       </c>
       <c r="E35" s="33" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F35" s="33" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="G35" s="33"/>
       <c r="H35" s="33"/>
@@ -3743,62 +4041,58 @@
       </c>
     </row>
     <row r="36" spans="1:15">
-      <c r="K36" s="53"/>
-    </row>
-    <row r="38" spans="1:15" ht="20.25">
-      <c r="A38" s="19" t="s">
+      <c r="A36" s="40">
+        <v>4</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="C36" s="41" t="s">
+        <v>265</v>
+      </c>
+      <c r="D36" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="F36" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="52" t="s">
+        <v>263</v>
+      </c>
+      <c r="K36" s="53" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="K37" s="53"/>
+    </row>
+    <row r="39" spans="1:15" ht="20.25">
+      <c r="A39" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-    </row>
-    <row r="39" spans="1:15">
-      <c r="A39" s="53">
-        <v>1</v>
-      </c>
-      <c r="B39" s="53" t="s">
-        <v>276</v>
-      </c>
-      <c r="C39" s="53" t="s">
-        <v>277</v>
-      </c>
-      <c r="D39" s="53" t="s">
-        <v>278</v>
-      </c>
-      <c r="E39" s="53" t="s">
-        <v>279</v>
-      </c>
-      <c r="F39" s="53" t="s">
-        <v>280</v>
-      </c>
-      <c r="G39" s="53"/>
-      <c r="H39" s="53"/>
-      <c r="I39" s="67"/>
-      <c r="J39" s="68" t="s">
-        <v>191</v>
-      </c>
-      <c r="K39" s="53" t="s">
-        <v>221</v>
-      </c>
-      <c r="L39" s="28"/>
-      <c r="M39" s="28"/>
-      <c r="N39" s="22"/>
-      <c r="O39" s="22"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B40" s="53" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C40" s="53" t="s">
         <v>277</v>
@@ -3807,7 +4101,7 @@
         <v>278</v>
       </c>
       <c r="E40" s="53" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F40" s="53" t="s">
         <v>280</v>
@@ -3815,70 +4109,70 @@
       <c r="G40" s="53"/>
       <c r="H40" s="53"/>
       <c r="I40" s="67"/>
-      <c r="J40" s="69" t="s">
+      <c r="J40" s="68" t="s">
         <v>191</v>
       </c>
       <c r="K40" s="53" t="s">
         <v>221</v>
       </c>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
       <c r="N40" s="22"/>
       <c r="O40" s="22"/>
     </row>
     <row r="41" spans="1:15">
-      <c r="A41" s="33">
-        <v>3</v>
-      </c>
-      <c r="B41" s="33" t="s">
-        <v>283</v>
-      </c>
-      <c r="C41" s="33" t="s">
-        <v>284</v>
-      </c>
-      <c r="D41" s="33" t="s">
+      <c r="A41" s="53">
+        <v>2</v>
+      </c>
+      <c r="B41" s="53" t="s">
+        <v>281</v>
+      </c>
+      <c r="C41" s="53" t="s">
+        <v>277</v>
+      </c>
+      <c r="D41" s="53" t="s">
         <v>278</v>
       </c>
-      <c r="E41" s="33" t="s">
-        <v>285</v>
-      </c>
-      <c r="F41" s="33" t="s">
-        <v>286</v>
-      </c>
-      <c r="G41" s="33"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="34"/>
+      <c r="E41" s="53" t="s">
+        <v>282</v>
+      </c>
+      <c r="F41" s="53" t="s">
+        <v>280</v>
+      </c>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="67"/>
       <c r="J41" s="69" t="s">
         <v>191</v>
       </c>
       <c r="K41" s="53" t="s">
         <v>221</v>
       </c>
-      <c r="L41" s="22"/>
-      <c r="M41" s="22"/>
+      <c r="L41" s="29"/>
+      <c r="M41" s="29"/>
       <c r="N41" s="22"/>
       <c r="O41" s="22"/>
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B42" s="33" t="s">
-        <v>287</v>
-      </c>
-      <c r="C42" s="53" t="s">
-        <v>288</v>
-      </c>
-      <c r="D42" s="53" t="s">
+        <v>283</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="D42" s="33" t="s">
         <v>278</v>
       </c>
-      <c r="E42" s="53" t="s">
-        <v>289</v>
+      <c r="E42" s="33" t="s">
+        <v>285</v>
       </c>
       <c r="F42" s="33" t="s">
-        <v>290</v>
-      </c>
-      <c r="G42" s="53"/>
+        <v>286</v>
+      </c>
+      <c r="G42" s="33"/>
       <c r="H42" s="33"/>
       <c r="I42" s="34"/>
       <c r="J42" s="69" t="s">
@@ -3894,10 +4188,10 @@
     </row>
     <row r="43" spans="1:15">
       <c r="A43" s="33">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C43" s="53" t="s">
         <v>288</v>
@@ -3906,9 +4200,9 @@
         <v>278</v>
       </c>
       <c r="E43" s="53" t="s">
-        <v>292</v>
-      </c>
-      <c r="F43" s="53" t="s">
+        <v>289</v>
+      </c>
+      <c r="F43" s="33" t="s">
         <v>290</v>
       </c>
       <c r="G43" s="53"/>
@@ -3925,14 +4219,26 @@
       <c r="N43" s="22"/>
       <c r="O43" s="22"/>
     </row>
-    <row r="44" spans="1:15" ht="17.25">
-      <c r="A44" s="33"/>
-      <c r="B44" s="70"/>
-      <c r="C44" s="33"/>
-      <c r="D44" s="33"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="33"/>
+    <row r="44" spans="1:15">
+      <c r="A44" s="33">
+        <v>5</v>
+      </c>
+      <c r="B44" s="33" t="s">
+        <v>291</v>
+      </c>
+      <c r="C44" s="53" t="s">
+        <v>288</v>
+      </c>
+      <c r="D44" s="53" t="s">
+        <v>278</v>
+      </c>
+      <c r="E44" s="53" t="s">
+        <v>292</v>
+      </c>
+      <c r="F44" s="53" t="s">
+        <v>290</v>
+      </c>
+      <c r="G44" s="53"/>
       <c r="H44" s="33"/>
       <c r="I44" s="34"/>
       <c r="J44" s="69" t="s">
@@ -3946,25 +4252,13 @@
       <c r="N44" s="22"/>
       <c r="O44" s="22"/>
     </row>
-    <row r="45" spans="1:15">
-      <c r="A45" s="33">
-        <v>6</v>
-      </c>
-      <c r="B45" s="33" t="s">
-        <v>293</v>
-      </c>
-      <c r="C45" s="53" t="s">
-        <v>294</v>
-      </c>
-      <c r="D45" s="53" t="s">
-        <v>278</v>
-      </c>
-      <c r="E45" s="53" t="s">
-        <v>295</v>
-      </c>
-      <c r="F45" s="53" t="s">
-        <v>296</v>
-      </c>
+    <row r="45" spans="1:15" ht="17.25">
+      <c r="A45" s="33"/>
+      <c r="B45" s="70"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
       <c r="G45" s="33"/>
       <c r="H45" s="33"/>
       <c r="I45" s="34"/>
@@ -3981,51 +4275,57 @@
     </row>
     <row r="46" spans="1:15">
       <c r="A46" s="33">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B46" s="33" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C46" s="53" t="s">
-        <v>298</v>
-      </c>
-      <c r="D46" s="33" t="s">
+        <v>294</v>
+      </c>
+      <c r="D46" s="53" t="s">
         <v>278</v>
       </c>
-      <c r="E46" s="33" t="s">
-        <v>299</v>
-      </c>
-      <c r="F46" s="33" t="s">
+      <c r="E46" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="F46" s="53" t="s">
         <v>296</v>
       </c>
       <c r="G46" s="33"/>
       <c r="H46" s="33"/>
       <c r="I46" s="34"/>
-      <c r="J46" s="33"/>
+      <c r="J46" s="69" t="s">
+        <v>191</v>
+      </c>
       <c r="K46" s="53" t="s">
         <v>221</v>
       </c>
+      <c r="L46" s="22"/>
+      <c r="M46" s="22"/>
+      <c r="N46" s="22"/>
+      <c r="O46" s="22"/>
     </row>
     <row r="47" spans="1:15">
       <c r="A47" s="33">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B47" s="33" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C47" s="53" t="s">
-        <v>301</v>
-      </c>
-      <c r="D47" s="53" t="s">
+        <v>298</v>
+      </c>
+      <c r="D47" s="33" t="s">
         <v>278</v>
       </c>
-      <c r="E47" s="53" t="s">
-        <v>302</v>
+      <c r="E47" s="33" t="s">
+        <v>299</v>
       </c>
       <c r="F47" s="33" t="s">
-        <v>303</v>
-      </c>
-      <c r="G47" s="53"/>
+        <v>296</v>
+      </c>
+      <c r="G47" s="33"/>
       <c r="H47" s="33"/>
       <c r="I47" s="34"/>
       <c r="J47" s="33"/>
@@ -4033,81 +4333,774 @@
         <v>221</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="23.25">
-      <c r="A49" s="24" t="s">
+    <row r="48" spans="1:15">
+      <c r="A48" s="33">
+        <v>8</v>
+      </c>
+      <c r="B48" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="C48" s="53" t="s">
+        <v>301</v>
+      </c>
+      <c r="D48" s="53" t="s">
+        <v>278</v>
+      </c>
+      <c r="E48" s="53" t="s">
+        <v>302</v>
+      </c>
+      <c r="F48" s="33" t="s">
+        <v>303</v>
+      </c>
+      <c r="G48" s="53"/>
+      <c r="H48" s="33"/>
+      <c r="I48" s="34"/>
+      <c r="J48" s="33"/>
+      <c r="K48" s="53" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="23.25">
+      <c r="A50" s="24" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
-      <c r="A50" s="43">
+    <row r="51" spans="1:11">
+      <c r="A51" s="43">
         <v>1</v>
       </c>
-      <c r="B50" s="43" t="s">
+      <c r="B51" s="43" t="s">
         <v>305</v>
       </c>
-      <c r="C50" s="50" t="s">
+      <c r="C51" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="D50" s="43" t="s">
+      <c r="D51" s="43" t="s">
         <v>307</v>
       </c>
-      <c r="E50" s="43" t="s">
+      <c r="E51" s="43" t="s">
         <v>308</v>
       </c>
-      <c r="F50" s="43" t="s">
+      <c r="F51" s="43" t="s">
         <v>309</v>
       </c>
-      <c r="G50" s="43" t="s">
+      <c r="G51" s="43" t="s">
         <v>310</v>
       </c>
-      <c r="H50" s="43"/>
-      <c r="I50" s="46"/>
-      <c r="J50" s="43"/>
-      <c r="K50" s="43"/>
-    </row>
-    <row r="51" spans="1:11">
-      <c r="B51" s="36" t="s">
+      <c r="H51" s="43"/>
+      <c r="I51" s="46"/>
+      <c r="J51" s="43"/>
+      <c r="K51" s="43"/>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="B52" s="36" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
-      <c r="B52" s="43" t="s">
+    <row r="53" spans="1:11">
+      <c r="B53" s="43" t="s">
         <v>312</v>
       </c>
-      <c r="C52" s="43"/>
-      <c r="D52" s="43"/>
-      <c r="E52" s="43"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="43"/>
-      <c r="H52" s="43"/>
-      <c r="I52" s="46"/>
-      <c r="J52" s="43"/>
-      <c r="K52" s="43"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="43"/>
+      <c r="E53" s="43"/>
+      <c r="F53" s="43"/>
+      <c r="G53" s="43"/>
+      <c r="H53" s="43"/>
+      <c r="I53" s="46"/>
+      <c r="J53" s="43"/>
+      <c r="K53" s="43"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C12" r:id="rId1" location=".VrNcerKLTIW" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="C13" r:id="rId2" location=".VrNcerKLTIW" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="C16" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="C20" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="C21" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink ref="C22" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
-    <hyperlink ref="C23" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
-    <hyperlink ref="C24" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
-    <hyperlink ref="C25" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
-    <hyperlink ref="C26" r:id="rId10" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
-    <hyperlink ref="C28" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
-    <hyperlink ref="C29" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
-    <hyperlink ref="C30" r:id="rId13" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
-    <hyperlink ref="C32" r:id="rId14" xr:uid="{00000000-0004-0000-0300-00000E000000}"/>
-    <hyperlink ref="C33" r:id="rId15" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
-    <hyperlink ref="C34" r:id="rId16" xr:uid="{00000000-0004-0000-0300-000010000000}"/>
-    <hyperlink ref="C35" r:id="rId17" xr:uid="{00000000-0004-0000-0300-000011000000}"/>
-    <hyperlink ref="C11" r:id="rId18" location=".VrNcerKLTIW" xr:uid="{21DECC9C-47EC-44BE-9F30-A266B2D261DB}"/>
+    <hyperlink ref="C12" r:id="rId1" location=".VrNcerKLTIW"/>
+    <hyperlink ref="C13" r:id="rId2" location=".VrNcerKLTIW"/>
+    <hyperlink ref="C16" r:id="rId3"/>
+    <hyperlink ref="C20" r:id="rId4"/>
+    <hyperlink ref="C21" r:id="rId5"/>
+    <hyperlink ref="C22" r:id="rId6"/>
+    <hyperlink ref="C23" r:id="rId7"/>
+    <hyperlink ref="C24" r:id="rId8"/>
+    <hyperlink ref="C25" r:id="rId9"/>
+    <hyperlink ref="C26" r:id="rId10"/>
+    <hyperlink ref="C28" r:id="rId11"/>
+    <hyperlink ref="C29" r:id="rId12"/>
+    <hyperlink ref="C30" r:id="rId13"/>
+    <hyperlink ref="C33" r:id="rId14"/>
+    <hyperlink ref="C34" r:id="rId15"/>
+    <hyperlink ref="C35" r:id="rId16"/>
+    <hyperlink ref="C36" r:id="rId17"/>
+    <hyperlink ref="C11" r:id="rId18" location=".VrNcerKLTIW"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="4" max="1048575" man="1"/>
+  </colBreaks>
   <legacyDrawing r:id="rId20"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="58.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="64" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="30">
+      <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="L1" s="31"/>
+    </row>
+    <row r="2" spans="1:13" ht="20.25">
+      <c r="A2" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="I2" s="14"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.75">
+      <c r="A3" s="84" t="s">
+        <v>336</v>
+      </c>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:13" s="72" customFormat="1">
+      <c r="A4" s="72">
+        <v>1</v>
+      </c>
+      <c r="B4" s="72" t="s">
+        <v>339</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="72" t="s">
+        <v>323</v>
+      </c>
+      <c r="E4" s="72" t="s">
+        <v>358</v>
+      </c>
+      <c r="F4" s="72" t="s">
+        <v>374</v>
+      </c>
+      <c r="G4" s="72" t="s">
+        <v>366</v>
+      </c>
+      <c r="K4" s="76" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="72" customFormat="1">
+      <c r="A5" s="72">
+        <v>2</v>
+      </c>
+      <c r="B5" s="72" t="s">
+        <v>340</v>
+      </c>
+      <c r="C5" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="72" t="s">
+        <v>323</v>
+      </c>
+      <c r="E5" s="72" t="s">
+        <v>359</v>
+      </c>
+      <c r="F5" s="72" t="s">
+        <v>375</v>
+      </c>
+      <c r="G5" s="72" t="s">
+        <v>367</v>
+      </c>
+      <c r="K5" s="76" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="72" customFormat="1" ht="30">
+      <c r="A6" s="71">
+        <v>3</v>
+      </c>
+      <c r="B6" s="72" t="s">
+        <v>326</v>
+      </c>
+      <c r="C6" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="72" t="s">
+        <v>323</v>
+      </c>
+      <c r="E6" s="72" t="s">
+        <v>360</v>
+      </c>
+      <c r="F6" s="78" t="s">
+        <v>372</v>
+      </c>
+      <c r="G6" s="72" t="s">
+        <v>327</v>
+      </c>
+      <c r="J6" s="75"/>
+      <c r="K6" s="76" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="72" customFormat="1" ht="30">
+      <c r="A7" s="71">
+        <v>4</v>
+      </c>
+      <c r="B7" s="72" t="s">
+        <v>322</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="72" t="s">
+        <v>323</v>
+      </c>
+      <c r="E7" s="72" t="s">
+        <v>361</v>
+      </c>
+      <c r="F7" s="74" t="s">
+        <v>373</v>
+      </c>
+      <c r="G7" s="72" t="s">
+        <v>324</v>
+      </c>
+      <c r="H7" s="77"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="76" t="s">
+        <v>321</v>
+      </c>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+    </row>
+    <row r="8" spans="1:13" s="72" customFormat="1">
+      <c r="A8" s="85">
+        <v>5</v>
+      </c>
+      <c r="B8" s="72" t="s">
+        <v>341</v>
+      </c>
+      <c r="C8" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="72" t="s">
+        <v>323</v>
+      </c>
+      <c r="E8" s="72" t="s">
+        <v>362</v>
+      </c>
+      <c r="F8" s="72" t="s">
+        <v>376</v>
+      </c>
+      <c r="G8" s="72" t="s">
+        <v>368</v>
+      </c>
+      <c r="K8" s="76" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="72" customFormat="1">
+      <c r="A9" s="85">
+        <v>6</v>
+      </c>
+      <c r="B9" s="72" t="s">
+        <v>342</v>
+      </c>
+      <c r="C9" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="72" t="s">
+        <v>323</v>
+      </c>
+      <c r="E9" s="72" t="s">
+        <v>363</v>
+      </c>
+      <c r="F9" s="72" t="s">
+        <v>377</v>
+      </c>
+      <c r="G9" s="72" t="s">
+        <v>369</v>
+      </c>
+      <c r="K9" s="76" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="72" customFormat="1">
+      <c r="A10" s="85">
+        <v>7</v>
+      </c>
+      <c r="B10" s="72" t="s">
+        <v>343</v>
+      </c>
+      <c r="C10" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="72" t="s">
+        <v>323</v>
+      </c>
+      <c r="E10" s="72" t="s">
+        <v>364</v>
+      </c>
+      <c r="F10" s="72" t="s">
+        <v>378</v>
+      </c>
+      <c r="G10" s="72" t="s">
+        <v>370</v>
+      </c>
+      <c r="K10" s="76" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="72" customFormat="1" ht="30">
+      <c r="A11" s="72">
+        <v>8</v>
+      </c>
+      <c r="B11" s="72" t="s">
+        <v>344</v>
+      </c>
+      <c r="C11" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="72" t="s">
+        <v>323</v>
+      </c>
+      <c r="E11" s="72" t="s">
+        <v>365</v>
+      </c>
+      <c r="F11" s="74" t="s">
+        <v>379</v>
+      </c>
+      <c r="G11" s="72" t="s">
+        <v>371</v>
+      </c>
+      <c r="H11" s="77"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="76" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75">
+      <c r="A12" s="84" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="72" customFormat="1">
+      <c r="A13" s="72">
+        <v>1</v>
+      </c>
+      <c r="B13" s="72" t="s">
+        <v>345</v>
+      </c>
+      <c r="C13" s="73" t="s">
+        <v>229</v>
+      </c>
+      <c r="D13" s="72" t="s">
+        <v>357</v>
+      </c>
+      <c r="E13" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="72" t="s">
+        <v>395</v>
+      </c>
+      <c r="G13" s="72" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="72" customFormat="1">
+      <c r="A14" s="72">
+        <v>2</v>
+      </c>
+      <c r="B14" s="72" t="s">
+        <v>346</v>
+      </c>
+      <c r="C14" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="72" t="s">
+        <v>357</v>
+      </c>
+      <c r="E14" s="72" t="s">
+        <v>380</v>
+      </c>
+      <c r="F14" s="72" t="s">
+        <v>396</v>
+      </c>
+      <c r="G14" s="72" t="s">
+        <v>388</v>
+      </c>
+      <c r="K14" s="76" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="72" customFormat="1">
+      <c r="A15" s="72">
+        <v>3</v>
+      </c>
+      <c r="B15" s="72" t="s">
+        <v>347</v>
+      </c>
+      <c r="C15" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="72" t="s">
+        <v>357</v>
+      </c>
+      <c r="E15" s="72" t="s">
+        <v>381</v>
+      </c>
+      <c r="F15" s="72" t="s">
+        <v>397</v>
+      </c>
+      <c r="G15" s="72" t="s">
+        <v>389</v>
+      </c>
+      <c r="K15" s="76" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="72" customFormat="1">
+      <c r="A16" s="72">
+        <v>4</v>
+      </c>
+      <c r="B16" s="72" t="s">
+        <v>348</v>
+      </c>
+      <c r="C16" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="72" t="s">
+        <v>357</v>
+      </c>
+      <c r="E16" s="72" t="s">
+        <v>382</v>
+      </c>
+      <c r="F16" s="72" t="s">
+        <v>398</v>
+      </c>
+      <c r="G16" s="72" t="s">
+        <v>390</v>
+      </c>
+      <c r="K16" s="76" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="72" customFormat="1">
+      <c r="A17" s="72">
+        <v>5</v>
+      </c>
+      <c r="B17" s="72" t="s">
+        <v>349</v>
+      </c>
+      <c r="C17" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="72" t="s">
+        <v>357</v>
+      </c>
+      <c r="E17" s="72" t="s">
+        <v>383</v>
+      </c>
+      <c r="F17" s="72" t="s">
+        <v>399</v>
+      </c>
+      <c r="G17" s="72" t="s">
+        <v>391</v>
+      </c>
+      <c r="K17" s="76" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="72" customFormat="1">
+      <c r="A18" s="72">
+        <v>6</v>
+      </c>
+      <c r="B18" s="72" t="s">
+        <v>350</v>
+      </c>
+      <c r="C18" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="72" t="s">
+        <v>357</v>
+      </c>
+      <c r="E18" s="72" t="s">
+        <v>384</v>
+      </c>
+      <c r="F18" s="72" t="s">
+        <v>400</v>
+      </c>
+      <c r="G18" s="72" t="s">
+        <v>392</v>
+      </c>
+      <c r="K18" s="76" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="72" customFormat="1">
+      <c r="A19" s="72">
+        <v>7</v>
+      </c>
+      <c r="B19" s="72" t="s">
+        <v>351</v>
+      </c>
+      <c r="C19" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="72" t="s">
+        <v>357</v>
+      </c>
+      <c r="E19" s="72" t="s">
+        <v>385</v>
+      </c>
+      <c r="F19" s="72" t="s">
+        <v>401</v>
+      </c>
+      <c r="G19" s="72" t="s">
+        <v>393</v>
+      </c>
+      <c r="K19" s="76" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="72" customFormat="1">
+      <c r="A20" s="72">
+        <v>8</v>
+      </c>
+      <c r="B20" s="72" t="s">
+        <v>352</v>
+      </c>
+      <c r="C20" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="72" t="s">
+        <v>357</v>
+      </c>
+      <c r="E20" s="72" t="s">
+        <v>386</v>
+      </c>
+      <c r="F20" s="72" t="s">
+        <v>402</v>
+      </c>
+      <c r="G20" s="72" t="s">
+        <v>394</v>
+      </c>
+      <c r="K20" s="76" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75">
+      <c r="A21" s="84" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="72" customFormat="1" ht="30">
+      <c r="A22" s="71">
+        <v>1</v>
+      </c>
+      <c r="B22" s="72" t="s">
+        <v>317</v>
+      </c>
+      <c r="C22" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="72" t="s">
+        <v>316</v>
+      </c>
+      <c r="E22" s="72" t="s">
+        <v>403</v>
+      </c>
+      <c r="F22" s="72" t="s">
+        <v>318</v>
+      </c>
+      <c r="G22" s="72" t="s">
+        <v>319</v>
+      </c>
+      <c r="I22" s="74" t="s">
+        <v>320</v>
+      </c>
+      <c r="J22" s="75"/>
+      <c r="K22" s="76" t="s">
+        <v>321</v>
+      </c>
+      <c r="L22" s="75"/>
+      <c r="M22" s="75"/>
+    </row>
+    <row r="23" spans="1:13" s="72" customFormat="1">
+      <c r="A23" s="71">
+        <v>2</v>
+      </c>
+      <c r="B23" s="72" t="s">
+        <v>353</v>
+      </c>
+      <c r="C23" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="72" t="s">
+        <v>316</v>
+      </c>
+      <c r="E23" s="72" t="s">
+        <v>404</v>
+      </c>
+      <c r="F23" s="72" t="s">
+        <v>408</v>
+      </c>
+      <c r="I23" s="74"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="76"/>
+      <c r="L23" s="75"/>
+      <c r="M23" s="75"/>
+    </row>
+    <row r="24" spans="1:13" s="72" customFormat="1" ht="30">
+      <c r="A24" s="72">
+        <v>3</v>
+      </c>
+      <c r="B24" s="72" t="s">
+        <v>354</v>
+      </c>
+      <c r="C24" s="73" t="s">
+        <v>313</v>
+      </c>
+      <c r="D24" s="72" t="s">
+        <v>316</v>
+      </c>
+      <c r="E24" s="72" t="s">
+        <v>405</v>
+      </c>
+      <c r="F24" s="72" t="s">
+        <v>331</v>
+      </c>
+      <c r="G24" s="72" t="s">
+        <v>332</v>
+      </c>
+      <c r="H24" s="77"/>
+      <c r="I24" s="74" t="s">
+        <v>329</v>
+      </c>
+      <c r="J24" s="75"/>
+      <c r="K24" s="72" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="72" customFormat="1" ht="30">
+      <c r="A25" s="72">
+        <v>4</v>
+      </c>
+      <c r="B25" s="72" t="s">
+        <v>355</v>
+      </c>
+      <c r="C25" s="73" t="s">
+        <v>313</v>
+      </c>
+      <c r="D25" s="72" t="s">
+        <v>316</v>
+      </c>
+      <c r="E25" s="72" t="s">
+        <v>406</v>
+      </c>
+      <c r="F25" s="72" t="s">
+        <v>333</v>
+      </c>
+      <c r="G25" s="72" t="s">
+        <v>328</v>
+      </c>
+      <c r="H25" s="77"/>
+      <c r="I25" s="74" t="s">
+        <v>329</v>
+      </c>
+      <c r="J25" s="75"/>
+      <c r="K25" s="72" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="72" customFormat="1" ht="30">
+      <c r="A26" s="72">
+        <v>5</v>
+      </c>
+      <c r="B26" s="72" t="s">
+        <v>356</v>
+      </c>
+      <c r="C26" s="73" t="s">
+        <v>314</v>
+      </c>
+      <c r="D26" s="72" t="s">
+        <v>316</v>
+      </c>
+      <c r="E26" s="72" t="s">
+        <v>407</v>
+      </c>
+      <c r="F26" s="72" t="s">
+        <v>335</v>
+      </c>
+      <c r="G26" s="72" t="s">
+        <v>334</v>
+      </c>
+      <c r="H26" s="77"/>
+      <c r="I26" s="74" t="s">
+        <v>329</v>
+      </c>
+      <c r="J26" s="75"/>
+      <c r="K26" s="72" t="s">
+        <v>315</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C13" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4352,13 +5345,38 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB7ADA5B-1C79-422C-B3D8-5CED891E2FC0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB7ADA5B-1C79-422C-B3D8-5CED891E2FC0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="edfacf83-951b-4dc6-822b-2c02bca35ad8"/>
+    <ds:schemaRef ds:uri="06e0d976-3d31-4bf3-b229-12f0909620f9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1149C42-F0A2-43BA-9A37-66E82BA50BBA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1149C42-F0A2-43BA-9A37-66E82BA50BBA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{565A1A7D-0DB7-49F9-A787-5BF8A5576797}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{565A1A7D-0DB7-49F9-A787-5BF8A5576797}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="06e0d976-3d31-4bf3-b229-12f0909620f9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix employ sector and services charts
</commit_message>
<xml_diff>
--- a/docs/DCD_DataSheet.xlsx
+++ b/docs/DCD_DataSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22420" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="960" yWindow="-20540" windowWidth="38400" windowHeight="20540" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Landing Page" sheetId="2" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="315">
   <si>
     <t>Card</t>
   </si>
@@ -1066,10 +1066,7 @@
     <t>http://www.dublindashboard.ie/DublinEconomicMon/stats</t>
   </si>
   <si>
-    <t>links broekn</t>
-  </si>
-  <si>
-    <t>links broekn (acc disabled)</t>
+    <t>Broad sector data only available for short time, file needs a line of processing manually</t>
   </si>
 </sst>
 </file>
@@ -1303,7 +1300,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1394,12 +1391,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1440,7 +1431,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -1586,18 +1577,15 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="60% - Accent6" xfId="6" builtinId="52"/>
@@ -2949,8 +2937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4111,7 +4099,7 @@
       <c r="I48" s="31"/>
       <c r="J48" s="51"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="31"/>
       <c r="B49" s="31"/>
       <c r="C49" s="51"/>
@@ -4123,96 +4111,95 @@
       <c r="I49" s="31"/>
       <c r="J49" s="51"/>
     </row>
-    <row r="50" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="90"/>
-      <c r="B50" s="91" t="s">
+    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A50" s="87"/>
+      <c r="B50" s="88" t="s">
         <v>309</v>
       </c>
-      <c r="C50" s="87" t="s">
-        <v>315</v>
-      </c>
-      <c r="D50" s="92" t="s">
+      <c r="C50" s="74"/>
+      <c r="D50" s="89" t="s">
         <v>313</v>
       </c>
-      <c r="E50" s="88"/>
-      <c r="F50" s="87"/>
-      <c r="G50" s="88"/>
-      <c r="H50" s="89"/>
-      <c r="I50" s="88"/>
-      <c r="J50" s="87"/>
-    </row>
-    <row r="51" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="90"/>
-      <c r="B51" s="91" t="s">
+      <c r="E50" s="69"/>
+      <c r="F50" s="90"/>
+      <c r="G50" s="91"/>
+      <c r="H50" s="69"/>
+      <c r="I50" s="91"/>
+      <c r="J50" s="90"/>
+      <c r="K50" s="91"/>
+    </row>
+    <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A51" s="87"/>
+      <c r="B51" s="88" t="s">
         <v>310</v>
       </c>
-      <c r="C51" s="87" t="s">
+      <c r="C51" s="74"/>
+      <c r="D51" s="89" t="s">
+        <v>313</v>
+      </c>
+      <c r="E51" s="69" t="s">
         <v>314</v>
       </c>
-      <c r="D51" s="92" t="s">
+      <c r="F51" s="90"/>
+      <c r="G51" s="91"/>
+      <c r="H51" s="69"/>
+      <c r="I51" s="91"/>
+      <c r="J51" s="90"/>
+      <c r="K51" s="91"/>
+    </row>
+    <row r="52" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A52" s="87"/>
+      <c r="B52" s="88" t="s">
+        <v>311</v>
+      </c>
+      <c r="C52" s="74"/>
+      <c r="D52" s="89" t="s">
         <v>313</v>
       </c>
-      <c r="E51" s="88"/>
-      <c r="F51" s="87"/>
-      <c r="G51" s="88"/>
-      <c r="H51" s="89"/>
-      <c r="I51" s="88"/>
-      <c r="J51" s="87"/>
-    </row>
-    <row r="52" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="90"/>
-      <c r="B52" s="91" t="s">
-        <v>311</v>
-      </c>
-      <c r="C52" s="87" t="s">
-        <v>314</v>
-      </c>
-      <c r="D52" s="92" t="s">
+      <c r="E52" s="69"/>
+      <c r="F52" s="90"/>
+      <c r="G52" s="91"/>
+      <c r="H52" s="69"/>
+      <c r="I52" s="91"/>
+      <c r="J52" s="90"/>
+      <c r="K52" s="91"/>
+    </row>
+    <row r="53" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A53" s="87"/>
+      <c r="B53" s="88" t="s">
+        <v>312</v>
+      </c>
+      <c r="C53" s="74"/>
+      <c r="D53" s="89" t="s">
         <v>313</v>
       </c>
-      <c r="E52" s="88"/>
-      <c r="F52" s="87"/>
-      <c r="G52" s="88"/>
-      <c r="H52" s="89"/>
-      <c r="I52" s="88"/>
-      <c r="J52" s="87"/>
-    </row>
-    <row r="53" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="90"/>
-      <c r="B53" s="91" t="s">
-        <v>312</v>
-      </c>
-      <c r="C53" s="87" t="s">
-        <v>314</v>
-      </c>
-      <c r="D53" s="92" t="s">
-        <v>313</v>
-      </c>
-      <c r="E53" s="88"/>
-      <c r="F53" s="87"/>
-      <c r="G53" s="88"/>
-      <c r="H53" s="89"/>
-      <c r="I53" s="88"/>
-      <c r="J53" s="87"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A54" s="90"/>
-      <c r="B54" s="88"/>
-      <c r="C54" s="87"/>
-      <c r="D54" s="87"/>
-      <c r="E54" s="88"/>
-      <c r="F54" s="87"/>
-      <c r="G54" s="88"/>
-      <c r="H54" s="89"/>
-      <c r="I54" s="88"/>
-      <c r="J54" s="87"/>
-    </row>
-    <row r="56" spans="1:10" ht="24" x14ac:dyDescent="0.3">
+      <c r="E53" s="69"/>
+      <c r="F53" s="90"/>
+      <c r="G53" s="91"/>
+      <c r="H53" s="69"/>
+      <c r="I53" s="91"/>
+      <c r="J53" s="90"/>
+      <c r="K53" s="91"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" s="87"/>
+      <c r="B54" s="91"/>
+      <c r="C54" s="90"/>
+      <c r="D54" s="90"/>
+      <c r="E54" s="91"/>
+      <c r="F54" s="90"/>
+      <c r="G54" s="91"/>
+      <c r="H54" s="69"/>
+      <c r="I54" s="91"/>
+      <c r="J54" s="90"/>
+      <c r="K54" s="91"/>
+    </row>
+    <row r="56" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="A56" s="22" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="41">
         <v>1</v>
       </c>
@@ -4236,12 +4223,12 @@
       <c r="I57" s="41"/>
       <c r="J57" s="41"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B58" s="34" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B59" s="41" t="s">
         <v>306</v>
       </c>

</xml_diff>